<commit_message>
update Readme and introduce runCountSpores
</commit_message>
<xml_diff>
--- a/Data_analysis/data_prop_long.xlsx
+++ b/Data_analysis/data_prop_long.xlsx
@@ -6,9 +6,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LD" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="GA3" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="ABA" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="GA3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="LD" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Day</t>
   </si>
   <si>
-    <t xml:space="preserve">Fragment</t>
+    <t xml:space="preserve">Segment</t>
   </si>
   <si>
     <t xml:space="preserve">Proportion</t>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">Prop1</t>
+    <t xml:space="preserve">Prop_1</t>
   </si>
   <si>
     <t xml:space="preserve">B</t>
@@ -73,10 +73,10 @@
     <t xml:space="preserve">9_14_DKO</t>
   </si>
   <si>
-    <t xml:space="preserve">Prop2</t>
+    <t xml:space="preserve">Prop_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Prop3</t>
+    <t xml:space="preserve">Prop_3</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="n">
-        <v>18.2134570765661</v>
+        <v>8.9943342776204</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -518,7 +518,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>93.7354988399072</v>
+        <v>15.1558073654391</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -550,7 +550,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>94.8955916473318</v>
+        <v>93.7677053824363</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
@@ -582,7 +582,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>97.7958236658933</v>
+        <v>94.3342776203966</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -614,7 +614,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>100</v>
+        <v>95.042492917847</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -710,7 +710,7 @@
         <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>18.2192910140148</v>
+        <v>21.583850931677</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -742,7 +742,7 @@
         <v>12</v>
       </c>
       <c r="E11" t="n">
-        <v>45.6718878812861</v>
+        <v>66.6149068322981</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
@@ -774,7 +774,7 @@
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>68.5902720527617</v>
+        <v>83.0745341614907</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
@@ -806,7 +806,7 @@
         <v>12</v>
       </c>
       <c r="E13" t="n">
-        <v>81.2860676009893</v>
+        <v>91.4596273291926</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -838,7 +838,7 @@
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>93.3223413025556</v>
+        <v>96.1180124223602</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -934,7 +934,7 @@
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>16.1073825503356</v>
+        <v>1.96850393700787</v>
       </c>
       <c r="F17" t="n">
         <v>1</v>
@@ -966,7 +966,7 @@
         <v>12</v>
       </c>
       <c r="E18" t="n">
-        <v>27.4651522973671</v>
+        <v>2.36220472440945</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
@@ -998,7 +998,7 @@
         <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>59.9380485286526</v>
+        <v>7.48031496062992</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
@@ -1030,7 +1030,7 @@
         <v>12</v>
       </c>
       <c r="E20" t="n">
-        <v>83.6344863190501</v>
+        <v>47.1128608923885</v>
       </c>
       <c r="F20" t="n">
         <v>1</v>
@@ -1062,7 +1062,7 @@
         <v>12</v>
       </c>
       <c r="E21" t="n">
-        <v>93.9597315436242</v>
+        <v>74.9343832020997</v>
       </c>
       <c r="F21" t="n">
         <v>1</v>
@@ -1094,7 +1094,7 @@
         <v>12</v>
       </c>
       <c r="E22" t="n">
-        <v>97.9349509550852</v>
+        <v>86.8766404199475</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
@@ -1158,7 +1158,7 @@
         <v>12</v>
       </c>
       <c r="E24" t="n">
-        <v>14.9615851192883</v>
+        <v>2.5944469731452</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -1190,7 +1190,7 @@
         <v>12</v>
       </c>
       <c r="E25" t="n">
-        <v>19.3691872219976</v>
+        <v>3.95994538006372</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -1222,7 +1222,7 @@
         <v>12</v>
       </c>
       <c r="E26" t="n">
-        <v>47.4727052163364</v>
+        <v>8.19299044151115</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -1254,7 +1254,7 @@
         <v>12</v>
       </c>
       <c r="E27" t="n">
-        <v>82.9761423372422</v>
+        <v>13.882567137005</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1286,7 +1286,7 @@
         <v>12</v>
       </c>
       <c r="E28" t="n">
-        <v>89.7290739991913</v>
+        <v>30.7692307692308</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1318,7 +1318,7 @@
         <v>12</v>
       </c>
       <c r="E29" t="n">
-        <v>97.9781641730691</v>
+        <v>43.468365953573</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -1382,7 +1382,7 @@
         <v>12</v>
       </c>
       <c r="E31" t="n">
-        <v>19.817439346625</v>
+        <v>14.931650893796</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -1414,7 +1414,7 @@
         <v>12</v>
       </c>
       <c r="E32" t="n">
-        <v>39.8750900792698</v>
+        <v>23.5541535226078</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -1446,7 +1446,7 @@
         <v>12</v>
       </c>
       <c r="E33" t="n">
-        <v>59.0439586836416</v>
+        <v>50.9989484752892</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1478,7 +1478,7 @@
         <v>12</v>
       </c>
       <c r="E34" t="n">
-        <v>70.9344222916166</v>
+        <v>78.7066246056782</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1510,7 +1510,7 @@
         <v>12</v>
       </c>
       <c r="E35" t="n">
-        <v>84.914724957963</v>
+        <v>87.0662460567823</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1542,7 +1542,7 @@
         <v>12</v>
       </c>
       <c r="E36" t="n">
-        <v>94.0427576267115</v>
+        <v>96.267087276551</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1606,7 +1606,7 @@
         <v>12</v>
       </c>
       <c r="E38" t="n">
-        <v>19.9732501114579</v>
+        <v>8.38654746700724</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1638,7 +1638,7 @@
         <v>12</v>
       </c>
       <c r="E39" t="n">
-        <v>62.9959875167187</v>
+        <v>22.3925074499787</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
@@ -1670,7 +1670,7 @@
         <v>12</v>
       </c>
       <c r="E40" t="n">
-        <v>97.9045920641997</v>
+        <v>41.8901660280971</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -1702,7 +1702,7 @@
         <v>12</v>
       </c>
       <c r="E41" t="n">
-        <v>98.4841729826126</v>
+        <v>65.6875266070668</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -1734,7 +1734,7 @@
         <v>12</v>
       </c>
       <c r="E42" t="n">
-        <v>98.4841729826126</v>
+        <v>83.1843337590464</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -1766,7 +1766,7 @@
         <v>12</v>
       </c>
       <c r="E43" t="n">
-        <v>100</v>
+        <v>86.6751809280545</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -1830,7 +1830,7 @@
         <v>12</v>
       </c>
       <c r="E45" t="n">
-        <v>23.9520958083832</v>
+        <v>22.972972972973</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1862,7 +1862,7 @@
         <v>12</v>
       </c>
       <c r="E46" t="n">
-        <v>65.9680638722555</v>
+        <v>74.0753911806543</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1894,7 +1894,7 @@
         <v>12</v>
       </c>
       <c r="E47" t="n">
-        <v>82.5349301397206</v>
+        <v>74.0753911806543</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -1926,7 +1926,7 @@
         <v>12</v>
       </c>
       <c r="E48" t="n">
-        <v>89.6207584830339</v>
+        <v>77.4893314366999</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -1958,7 +1958,7 @@
         <v>12</v>
       </c>
       <c r="E49" t="n">
-        <v>96.0079840319361</v>
+        <v>81.9701280227596</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -1990,7 +1990,7 @@
         <v>12</v>
       </c>
       <c r="E50" t="n">
-        <v>100</v>
+        <v>90.9672830725462</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
@@ -2054,7 +2054,7 @@
         <v>12</v>
       </c>
       <c r="E52" t="n">
-        <v>19.971671388102</v>
+        <v>14.2857142857143</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -2086,7 +2086,7 @@
         <v>12</v>
       </c>
       <c r="E53" t="n">
-        <v>79.1784702549575</v>
+        <v>71.865889212828</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -2118,7 +2118,7 @@
         <v>12</v>
       </c>
       <c r="E54" t="n">
-        <v>88.9518413597734</v>
+        <v>75.5102040816327</v>
       </c>
       <c r="F54" t="n">
         <v>0</v>
@@ -2150,7 +2150,7 @@
         <v>12</v>
       </c>
       <c r="E55" t="n">
-        <v>91.8555240793201</v>
+        <v>87.4635568513119</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
@@ -2182,7 +2182,7 @@
         <v>12</v>
       </c>
       <c r="E56" t="n">
-        <v>94.0509915014164</v>
+        <v>94.6064139941691</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
@@ -2214,7 +2214,7 @@
         <v>12</v>
       </c>
       <c r="E57" t="n">
-        <v>98.0878186968839</v>
+        <v>100</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
@@ -2278,7 +2278,7 @@
         <v>12</v>
       </c>
       <c r="E59" t="n">
-        <v>26.26953125</v>
+        <v>29.5936395759717</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
@@ -2310,7 +2310,7 @@
         <v>12</v>
       </c>
       <c r="E60" t="n">
-        <v>59.375</v>
+        <v>80.9628975265018</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
@@ -2342,7 +2342,7 @@
         <v>12</v>
       </c>
       <c r="E61" t="n">
-        <v>76.953125</v>
+        <v>89.2667844522968</v>
       </c>
       <c r="F61" t="n">
         <v>0</v>
@@ -2374,7 +2374,7 @@
         <v>12</v>
       </c>
       <c r="E62" t="n">
-        <v>87.109375</v>
+        <v>91.9611307420495</v>
       </c>
       <c r="F62" t="n">
         <v>0</v>
@@ -2406,7 +2406,7 @@
         <v>12</v>
       </c>
       <c r="E63" t="n">
-        <v>88.96484375</v>
+        <v>92.2703180212014</v>
       </c>
       <c r="F63" t="n">
         <v>0</v>
@@ -2438,7 +2438,7 @@
         <v>12</v>
       </c>
       <c r="E64" t="n">
-        <v>95.60546875</v>
+        <v>96.1572438162544</v>
       </c>
       <c r="F64" t="n">
         <v>0</v>
@@ -2502,7 +2502,7 @@
         <v>12</v>
       </c>
       <c r="E66" t="n">
-        <v>13.7733142037303</v>
+        <v>17.8705440900563</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
@@ -2534,7 +2534,7 @@
         <v>12</v>
       </c>
       <c r="E67" t="n">
-        <v>29.9856527977045</v>
+        <v>71.6228893058161</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
@@ -2566,7 +2566,7 @@
         <v>12</v>
       </c>
       <c r="E68" t="n">
-        <v>58.4791965566715</v>
+        <v>79.9718574108818</v>
       </c>
       <c r="F68" t="n">
         <v>0</v>
@@ -2598,7 +2598,7 @@
         <v>12</v>
       </c>
       <c r="E69" t="n">
-        <v>77.3027259684362</v>
+        <v>91.1350844277674</v>
       </c>
       <c r="F69" t="n">
         <v>0</v>
@@ -2630,7 +2630,7 @@
         <v>12</v>
       </c>
       <c r="E70" t="n">
-        <v>82.5824964131994</v>
+        <v>100</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
@@ -2662,7 +2662,7 @@
         <v>12</v>
       </c>
       <c r="E71" t="n">
-        <v>93.4863701578192</v>
+        <v>100</v>
       </c>
       <c r="F71" t="n">
         <v>0</v>
@@ -2726,7 +2726,7 @@
         <v>12</v>
       </c>
       <c r="E73" t="n">
-        <v>15.9838817998657</v>
+        <v>13.5854341736695</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
@@ -2758,7 +2758,7 @@
         <v>12</v>
       </c>
       <c r="E74" t="n">
-        <v>38.9858965748825</v>
+        <v>21.6736694677871</v>
       </c>
       <c r="F74" t="n">
         <v>0</v>
@@ -2790,7 +2790,7 @@
         <v>12</v>
       </c>
       <c r="E75" t="n">
-        <v>77.2666218938885</v>
+        <v>59.9789915966387</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
@@ -2822,7 +2822,7 @@
         <v>12</v>
       </c>
       <c r="E76" t="n">
-        <v>85.0906648757555</v>
+        <v>83.9985994397759</v>
       </c>
       <c r="F76" t="n">
         <v>0</v>
@@ -2854,7 +2854,7 @@
         <v>12</v>
       </c>
       <c r="E77" t="n">
-        <v>86.7696440564137</v>
+        <v>87.3949579831933</v>
       </c>
       <c r="F77" t="n">
         <v>0</v>
@@ -2886,7 +2886,7 @@
         <v>12</v>
       </c>
       <c r="E78" t="n">
-        <v>90.1947615849564</v>
+        <v>93.8725490196078</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
@@ -2950,7 +2950,7 @@
         <v>12</v>
       </c>
       <c r="E80" t="n">
-        <v>2.40096038415366</v>
+        <v>19.9920979849862</v>
       </c>
       <c r="F80" t="n">
         <v>0</v>
@@ -2982,7 +2982,7 @@
         <v>12</v>
       </c>
       <c r="E81" t="n">
-        <v>10.484193677471</v>
+        <v>53.0225207427894</v>
       </c>
       <c r="F81" t="n">
         <v>0</v>
@@ -3014,7 +3014,7 @@
         <v>12</v>
       </c>
       <c r="E82" t="n">
-        <v>42.6570628251301</v>
+        <v>68.4709600948242</v>
       </c>
       <c r="F82" t="n">
         <v>0</v>
@@ -3046,7 +3046,7 @@
         <v>12</v>
       </c>
       <c r="E83" t="n">
-        <v>63.1852741096439</v>
+        <v>77.3607269853813</v>
       </c>
       <c r="F83" t="n">
         <v>0</v>
@@ -3078,7 +3078,7 @@
         <v>12</v>
       </c>
       <c r="E84" t="n">
-        <v>72.9891956782713</v>
+        <v>85.7368629000395</v>
       </c>
       <c r="F84" t="n">
         <v>0</v>
@@ -3110,7 +3110,7 @@
         <v>12</v>
       </c>
       <c r="E85" t="n">
-        <v>89.9959983993597</v>
+        <v>91.2682734097195</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -3174,7 +3174,7 @@
         <v>12</v>
       </c>
       <c r="E87" t="n">
-        <v>40.9867784585618</v>
+        <v>25.7982120051086</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -3206,7 +3206,7 @@
         <v>12</v>
       </c>
       <c r="E88" t="n">
-        <v>92.9861335053209</v>
+        <v>89.9744572158365</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -3238,7 +3238,7 @@
         <v>12</v>
       </c>
       <c r="E89" t="n">
-        <v>95.6626894550145</v>
+        <v>93.3908045977011</v>
       </c>
       <c r="F89" t="n">
         <v>0</v>
@@ -3270,7 +3270,7 @@
         <v>12</v>
       </c>
       <c r="E90" t="n">
-        <v>95.9045469203483</v>
+        <v>94.5721583652618</v>
       </c>
       <c r="F90" t="n">
         <v>0</v>
@@ -3302,7 +3302,7 @@
         <v>12</v>
       </c>
       <c r="E91" t="n">
-        <v>96.0980328926153</v>
+        <v>96.9987228607918</v>
       </c>
       <c r="F91" t="n">
         <v>0</v>
@@ -3334,7 +3334,7 @@
         <v>12</v>
       </c>
       <c r="E92" t="n">
-        <v>100</v>
+        <v>97.57343550447</v>
       </c>
       <c r="F92" t="n">
         <v>0</v>
@@ -3398,7 +3398,7 @@
         <v>12</v>
       </c>
       <c r="E94" t="n">
-        <v>27.9881217520416</v>
+        <v>30.5336832895888</v>
       </c>
       <c r="F94" t="n">
         <v>0</v>
@@ -3430,7 +3430,7 @@
         <v>12</v>
       </c>
       <c r="E95" t="n">
-        <v>73.5708982925019</v>
+        <v>65.4418197725284</v>
       </c>
       <c r="F95" t="n">
         <v>0</v>
@@ -3462,7 +3462,7 @@
         <v>12</v>
       </c>
       <c r="E96" t="n">
-        <v>90.9428359317001</v>
+        <v>87.5765529308837</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
@@ -3494,7 +3494,7 @@
         <v>12</v>
       </c>
       <c r="E97" t="n">
-        <v>91.5738678544915</v>
+        <v>88.1889763779528</v>
       </c>
       <c r="F97" t="n">
         <v>0</v>
@@ -3526,7 +3526,7 @@
         <v>12</v>
       </c>
       <c r="E98" t="n">
-        <v>96.9933184855234</v>
+        <v>88.9763779527559</v>
       </c>
       <c r="F98" t="n">
         <v>0</v>
@@ -3558,7 +3558,7 @@
         <v>12</v>
       </c>
       <c r="E99" t="n">
-        <v>100</v>
+        <v>94.925634295713</v>
       </c>
       <c r="F99" t="n">
         <v>0</v>
@@ -3622,7 +3622,7 @@
         <v>12</v>
       </c>
       <c r="E101" t="n">
-        <v>21.9858156028369</v>
+        <v>22.3482699943279</v>
       </c>
       <c r="F101" t="n">
         <v>0</v>
@@ -3654,7 +3654,7 @@
         <v>12</v>
       </c>
       <c r="E102" t="n">
-        <v>80.2748226950355</v>
+        <v>70.5615428247306</v>
       </c>
       <c r="F102" t="n">
         <v>0</v>
@@ -3686,7 +3686,7 @@
         <v>12</v>
       </c>
       <c r="E103" t="n">
-        <v>91.6666666666667</v>
+        <v>81.5655133295519</v>
       </c>
       <c r="F103" t="n">
         <v>0</v>
@@ -3718,7 +3718,7 @@
         <v>12</v>
       </c>
       <c r="E104" t="n">
-        <v>92.9078014184397</v>
+        <v>91.26488939308</v>
       </c>
       <c r="F104" t="n">
         <v>0</v>
@@ -3750,7 +3750,7 @@
         <v>12</v>
       </c>
       <c r="E105" t="n">
-        <v>94.3262411347518</v>
+        <v>96.483267158253</v>
       </c>
       <c r="F105" t="n">
         <v>0</v>
@@ -3782,7 +3782,7 @@
         <v>12</v>
       </c>
       <c r="E106" t="n">
-        <v>100</v>
+        <v>98.1281905842314</v>
       </c>
       <c r="F106" t="n">
         <v>0</v>
@@ -3846,7 +3846,7 @@
         <v>19</v>
       </c>
       <c r="E108" t="n">
-        <v>18.0115273775216</v>
+        <v>9.29626411815812</v>
       </c>
       <c r="F108" t="n">
         <v>1</v>
@@ -3878,7 +3878,7 @@
         <v>19</v>
       </c>
       <c r="E109" t="n">
-        <v>92.3631123919308</v>
+        <v>15.2041702867072</v>
       </c>
       <c r="F109" t="n">
         <v>1</v>
@@ -3910,7 +3910,7 @@
         <v>19</v>
       </c>
       <c r="E110" t="n">
-        <v>95.6772334293948</v>
+        <v>94.1789748045178</v>
       </c>
       <c r="F110" t="n">
         <v>1</v>
@@ -3942,7 +3942,7 @@
         <v>19</v>
       </c>
       <c r="E111" t="n">
-        <v>97.8386167146974</v>
+        <v>94.7871416159861</v>
       </c>
       <c r="F111" t="n">
         <v>1</v>
@@ -3974,7 +3974,7 @@
         <v>19</v>
       </c>
       <c r="E112" t="n">
-        <v>100</v>
+        <v>95.4821894005213</v>
       </c>
       <c r="F112" t="n">
         <v>1</v>
@@ -4070,7 +4070,7 @@
         <v>19</v>
       </c>
       <c r="E115" t="n">
-        <v>18.7126741871267</v>
+        <v>22.2591362126246</v>
       </c>
       <c r="F115" t="n">
         <v>1</v>
@@ -4102,7 +4102,7 @@
         <v>19</v>
       </c>
       <c r="E116" t="n">
-        <v>49.6350364963504</v>
+        <v>65.2823920265781</v>
       </c>
       <c r="F116" t="n">
         <v>1</v>
@@ -4134,7 +4134,7 @@
         <v>19</v>
       </c>
       <c r="E117" t="n">
-        <v>66.9542136695421</v>
+        <v>85.0498338870432</v>
       </c>
       <c r="F117" t="n">
         <v>1</v>
@@ -4166,7 +4166,7 @@
         <v>19</v>
       </c>
       <c r="E118" t="n">
-        <v>81.8181818181818</v>
+        <v>90.0332225913621</v>
       </c>
       <c r="F118" t="n">
         <v>1</v>
@@ -4198,7 +4198,7 @@
         <v>19</v>
       </c>
       <c r="E119" t="n">
-        <v>92.9661579296616</v>
+        <v>97.0099667774086</v>
       </c>
       <c r="F119" t="n">
         <v>1</v>
@@ -4230,7 +4230,7 @@
         <v>19</v>
       </c>
       <c r="E120" t="n">
-        <v>99.535500995355</v>
+        <v>100</v>
       </c>
       <c r="F120" t="n">
         <v>1</v>
@@ -4294,7 +4294,7 @@
         <v>19</v>
       </c>
       <c r="E122" t="n">
-        <v>16.1499639509733</v>
+        <v>1.35135135135135</v>
       </c>
       <c r="F122" t="n">
         <v>1</v>
@@ -4326,7 +4326,7 @@
         <v>19</v>
       </c>
       <c r="E123" t="n">
-        <v>25.0180245133381</v>
+        <v>2.25225225225225</v>
       </c>
       <c r="F123" t="n">
         <v>1</v>
@@ -4358,7 +4358,7 @@
         <v>19</v>
       </c>
       <c r="E124" t="n">
-        <v>58.9762076423937</v>
+        <v>6.90690690690691</v>
       </c>
       <c r="F124" t="n">
         <v>1</v>
@@ -4390,7 +4390,7 @@
         <v>19</v>
       </c>
       <c r="E125" t="n">
-        <v>83.8500360490267</v>
+        <v>49.2492492492492</v>
       </c>
       <c r="F125" t="n">
         <v>1</v>
@@ -4422,7 +4422,7 @@
         <v>19</v>
       </c>
       <c r="E126" t="n">
-        <v>91.9250180245133</v>
+        <v>73.8738738738739</v>
       </c>
       <c r="F126" t="n">
         <v>1</v>
@@ -4454,7 +4454,7 @@
         <v>19</v>
       </c>
       <c r="E127" t="n">
-        <v>96.6834895457823</v>
+        <v>87.987987987988</v>
       </c>
       <c r="F127" t="n">
         <v>1</v>
@@ -4518,7 +4518,7 @@
         <v>19</v>
       </c>
       <c r="E129" t="n">
-        <v>15.0036954915004</v>
+        <v>2.00426439232409</v>
       </c>
       <c r="F129" t="n">
         <v>0</v>
@@ -4550,7 +4550,7 @@
         <v>19</v>
       </c>
       <c r="E130" t="n">
-        <v>18.0709534368071</v>
+        <v>4.26439232409382</v>
       </c>
       <c r="F130" t="n">
         <v>0</v>
@@ -4582,7 +4582,7 @@
         <v>19</v>
       </c>
       <c r="E131" t="n">
-        <v>52.069475240207</v>
+        <v>8.86993603411514</v>
       </c>
       <c r="F131" t="n">
         <v>0</v>
@@ -4614,7 +4614,7 @@
         <v>19</v>
       </c>
       <c r="E132" t="n">
-        <v>79.490022172949</v>
+        <v>13.8592750533049</v>
       </c>
       <c r="F132" t="n">
         <v>0</v>
@@ -4646,7 +4646,7 @@
         <v>19</v>
       </c>
       <c r="E133" t="n">
-        <v>90.5025868440503</v>
+        <v>31.4712153518124</v>
       </c>
       <c r="F133" t="n">
         <v>0</v>
@@ -4678,7 +4678,7 @@
         <v>19</v>
       </c>
       <c r="E134" t="n">
-        <v>94.9371766444937</v>
+        <v>45.6716417910448</v>
       </c>
       <c r="F134" t="n">
         <v>0</v>
@@ -4742,7 +4742,7 @@
         <v>19</v>
       </c>
       <c r="E136" t="n">
-        <v>22.4066390041494</v>
+        <v>13.376987839102</v>
       </c>
       <c r="F136" t="n">
         <v>0</v>
@@ -4774,7 +4774,7 @@
         <v>19</v>
       </c>
       <c r="E137" t="n">
-        <v>41.49377593361</v>
+        <v>24.7427502338634</v>
       </c>
       <c r="F137" t="n">
         <v>0</v>
@@ -4806,7 +4806,7 @@
         <v>19</v>
       </c>
       <c r="E138" t="n">
-        <v>54.1078838174274</v>
+        <v>50</v>
       </c>
       <c r="F138" t="n">
         <v>0</v>
@@ -4838,7 +4838,7 @@
         <v>19</v>
       </c>
       <c r="E139" t="n">
-        <v>65.9751037344398</v>
+        <v>80.355472404116</v>
       </c>
       <c r="F139" t="n">
         <v>0</v>
@@ -4870,7 +4870,7 @@
         <v>19</v>
       </c>
       <c r="E140" t="n">
-        <v>91.9087136929461</v>
+        <v>89.289055191768</v>
       </c>
       <c r="F140" t="n">
         <v>0</v>
@@ -4902,7 +4902,7 @@
         <v>19</v>
       </c>
       <c r="E141" t="n">
-        <v>89.9170124481328</v>
+        <v>95.3695042095416</v>
       </c>
       <c r="F141" t="n">
         <v>0</v>
@@ -4966,7 +4966,7 @@
         <v>19</v>
       </c>
       <c r="E143" t="n">
-        <v>28.0328480776409</v>
+        <v>7.87781350482315</v>
       </c>
       <c r="F143" t="n">
         <v>0</v>
@@ -4998,7 +4998,7 @@
         <v>19</v>
       </c>
       <c r="E144" t="n">
-        <v>64.9869354236655</v>
+        <v>23.9951768488746</v>
       </c>
       <c r="F144" t="n">
         <v>0</v>
@@ -5030,7 +5030,7 @@
         <v>19</v>
       </c>
       <c r="E145" t="n">
-        <v>95.9686450167973</v>
+        <v>41.5996784565916</v>
       </c>
       <c r="F145" t="n">
         <v>0</v>
@@ -5062,7 +5062,7 @@
         <v>19</v>
       </c>
       <c r="E146" t="n">
-        <v>96.7898469578201</v>
+        <v>66.7604501607717</v>
       </c>
       <c r="F146" t="n">
         <v>0</v>
@@ -5094,7 +5094,7 @@
         <v>19</v>
       </c>
       <c r="E147" t="n">
-        <v>96.7898469578201</v>
+        <v>84.5659163987138</v>
       </c>
       <c r="F147" t="n">
         <v>0</v>
@@ -5126,7 +5126,7 @@
         <v>19</v>
       </c>
       <c r="E148" t="n">
-        <v>100</v>
+        <v>86.2942122186495</v>
       </c>
       <c r="F148" t="n">
         <v>0</v>
@@ -5190,7 +5190,7 @@
         <v>19</v>
       </c>
       <c r="E150" t="n">
-        <v>21.9165085388994</v>
+        <v>22.3765996343693</v>
       </c>
       <c r="F150" t="n">
         <v>0</v>
@@ -5222,7 +5222,7 @@
         <v>19</v>
       </c>
       <c r="E151" t="n">
-        <v>66.7931688804554</v>
+        <v>75.2833638025594</v>
       </c>
       <c r="F151" t="n">
         <v>0</v>
@@ -5254,7 +5254,7 @@
         <v>19</v>
       </c>
       <c r="E152" t="n">
-        <v>82.9222011385199</v>
+        <v>75.2833638025594</v>
       </c>
       <c r="F152" t="n">
         <v>0</v>
@@ -5286,7 +5286,7 @@
         <v>19</v>
       </c>
       <c r="E153" t="n">
-        <v>87.4762808349146</v>
+        <v>78.2815356489945</v>
       </c>
       <c r="F153" t="n">
         <v>0</v>
@@ -5318,7 +5318,7 @@
         <v>19</v>
       </c>
       <c r="E154" t="n">
-        <v>91.8406072106262</v>
+        <v>81.3893967093236</v>
       </c>
       <c r="F154" t="n">
         <v>0</v>
@@ -5350,7 +5350,7 @@
         <v>19</v>
       </c>
       <c r="E155" t="n">
-        <v>100</v>
+        <v>90.164533820841</v>
       </c>
       <c r="F155" t="n">
         <v>0</v>
@@ -5414,7 +5414,7 @@
         <v>19</v>
       </c>
       <c r="E157" t="n">
-        <v>20.5699020480855</v>
+        <v>15.6706507304117</v>
       </c>
       <c r="F157" t="n">
         <v>0</v>
@@ -5446,7 +5446,7 @@
         <v>19</v>
       </c>
       <c r="E158" t="n">
-        <v>77.1148708815672</v>
+        <v>72.9083665338645</v>
       </c>
       <c r="F158" t="n">
         <v>0</v>
@@ -5478,7 +5478,7 @@
         <v>19</v>
       </c>
       <c r="E159" t="n">
-        <v>86.9991095280499</v>
+        <v>75.1660026560425</v>
       </c>
       <c r="F159" t="n">
         <v>0</v>
@@ -5510,7 +5510,7 @@
         <v>19</v>
       </c>
       <c r="E160" t="n">
-        <v>92.6090828138914</v>
+        <v>88.1806108897742</v>
       </c>
       <c r="F160" t="n">
         <v>0</v>
@@ -5542,7 +5542,7 @@
         <v>19</v>
       </c>
       <c r="E161" t="n">
-        <v>93.9447907390917</v>
+        <v>95.7503320053121</v>
       </c>
       <c r="F161" t="n">
         <v>0</v>
@@ -5574,7 +5574,7 @@
         <v>19</v>
       </c>
       <c r="E162" t="n">
-        <v>96.9723953695459</v>
+        <v>100</v>
       </c>
       <c r="F162" t="n">
         <v>0</v>
@@ -5638,7 +5638,7 @@
         <v>19</v>
       </c>
       <c r="E164" t="n">
-        <v>26.7206477732794</v>
+        <v>30.9668212629326</v>
       </c>
       <c r="F164" t="n">
         <v>0</v>
@@ -5670,7 +5670,7 @@
         <v>19</v>
       </c>
       <c r="E165" t="n">
-        <v>61.4372469635627</v>
+        <v>80.3781662504459</v>
       </c>
       <c r="F165" t="n">
         <v>0</v>
@@ -5702,7 +5702,7 @@
         <v>19</v>
       </c>
       <c r="E166" t="n">
-        <v>76.9230769230769</v>
+        <v>88.3696039957189</v>
       </c>
       <c r="F166" t="n">
         <v>0</v>
@@ -5734,7 +5734,7 @@
         <v>19</v>
       </c>
       <c r="E167" t="n">
-        <v>87.5506072874494</v>
+        <v>91.6874777024616</v>
       </c>
       <c r="F167" t="n">
         <v>0</v>
@@ -5766,7 +5766,7 @@
         <v>19</v>
       </c>
       <c r="E168" t="n">
-        <v>88.9676113360324</v>
+        <v>91.9728861933643</v>
       </c>
       <c r="F168" t="n">
         <v>0</v>
@@ -5798,7 +5798,7 @@
         <v>19</v>
       </c>
       <c r="E169" t="n">
-        <v>95.3441295546559</v>
+        <v>96.0756332500892</v>
       </c>
       <c r="F169" t="n">
         <v>0</v>
@@ -5862,7 +5862,7 @@
         <v>19</v>
       </c>
       <c r="E171" t="n">
-        <v>13.1161007667032</v>
+        <v>18.2905225863596</v>
       </c>
       <c r="F171" t="n">
         <v>0</v>
@@ -5894,7 +5894,7 @@
         <v>19</v>
       </c>
       <c r="E172" t="n">
-        <v>27.1084337349398</v>
+        <v>72.7635075287865</v>
       </c>
       <c r="F172" t="n">
         <v>0</v>
@@ -5926,7 +5926,7 @@
         <v>19</v>
       </c>
       <c r="E173" t="n">
-        <v>60.2135815991238</v>
+        <v>79.362267493357</v>
       </c>
       <c r="F173" t="n">
         <v>0</v>
@@ -5958,7 +5958,7 @@
         <v>19</v>
       </c>
       <c r="E174" t="n">
-        <v>76.7798466593647</v>
+        <v>90.4340124003543</v>
       </c>
       <c r="F174" t="n">
         <v>0</v>
@@ -5990,7 +5990,7 @@
         <v>19</v>
       </c>
       <c r="E175" t="n">
-        <v>82.9956188389923</v>
+        <v>100</v>
       </c>
       <c r="F175" t="n">
         <v>0</v>
@@ -6022,7 +6022,7 @@
         <v>19</v>
       </c>
       <c r="E176" t="n">
-        <v>92.579408543264</v>
+        <v>100</v>
       </c>
       <c r="F176" t="n">
         <v>0</v>
@@ -6086,7 +6086,7 @@
         <v>19</v>
       </c>
       <c r="E178" t="n">
-        <v>15.2752009894867</v>
+        <v>14.6772228989038</v>
       </c>
       <c r="F178" t="n">
         <v>0</v>
@@ -6118,7 +6118,7 @@
         <v>19</v>
       </c>
       <c r="E179" t="n">
-        <v>35.9925788497217</v>
+        <v>22.5943970767357</v>
       </c>
       <c r="F179" t="n">
         <v>0</v>
@@ -6150,7 +6150,7 @@
         <v>19</v>
       </c>
       <c r="E180" t="n">
-        <v>78.9734075448361</v>
+        <v>59.3788063337393</v>
       </c>
       <c r="F180" t="n">
         <v>0</v>
@@ -6182,7 +6182,7 @@
         <v>19</v>
       </c>
       <c r="E181" t="n">
-        <v>82.9931972789116</v>
+        <v>83.373934226553</v>
       </c>
       <c r="F181" t="n">
         <v>0</v>
@@ -6214,7 +6214,7 @@
         <v>19</v>
       </c>
       <c r="E182" t="n">
-        <v>86.2708719851577</v>
+        <v>88.5809987819732</v>
       </c>
       <c r="F182" t="n">
         <v>0</v>
@@ -6246,7 +6246,7 @@
         <v>19</v>
       </c>
       <c r="E183" t="n">
-        <v>88.9919604205318</v>
+        <v>91.5956151035323</v>
       </c>
       <c r="F183" t="n">
         <v>0</v>
@@ -6310,7 +6310,7 @@
         <v>19</v>
       </c>
       <c r="E185" t="n">
-        <v>4.88155061019383</v>
+        <v>19.5777351247601</v>
       </c>
       <c r="F185" t="n">
         <v>0</v>
@@ -6342,7 +6342,7 @@
         <v>19</v>
       </c>
       <c r="E186" t="n">
-        <v>12.275664034458</v>
+        <v>51.1996161228407</v>
       </c>
       <c r="F186" t="n">
         <v>0</v>
@@ -6374,7 +6374,7 @@
         <v>19</v>
       </c>
       <c r="E187" t="n">
-        <v>40.9906676238335</v>
+        <v>69.4817658349328</v>
       </c>
       <c r="F187" t="n">
         <v>0</v>
@@ -6406,7 +6406,7 @@
         <v>19</v>
       </c>
       <c r="E188" t="n">
-        <v>61.4860014357502</v>
+        <v>78.5988483685221</v>
       </c>
       <c r="F188" t="n">
         <v>0</v>
@@ -6438,7 +6438,7 @@
         <v>19</v>
       </c>
       <c r="E189" t="n">
-        <v>74.5872218234027</v>
+        <v>85.1727447216891</v>
       </c>
       <c r="F189" t="n">
         <v>0</v>
@@ -6470,7 +6470,7 @@
         <v>19</v>
       </c>
       <c r="E190" t="n">
-        <v>87.8679109834889</v>
+        <v>91.2667946257198</v>
       </c>
       <c r="F190" t="n">
         <v>0</v>
@@ -6534,7 +6534,7 @@
         <v>19</v>
       </c>
       <c r="E192" t="n">
-        <v>38.6872455902307</v>
+        <v>26.7925561029009</v>
       </c>
       <c r="F192" t="n">
         <v>0</v>
@@ -6566,7 +6566,7 @@
         <v>19</v>
       </c>
       <c r="E193" t="n">
-        <v>87.1947082767978</v>
+        <v>89.983579638752</v>
       </c>
       <c r="F193" t="n">
         <v>0</v>
@@ -6598,7 +6598,7 @@
         <v>19</v>
       </c>
       <c r="E194" t="n">
-        <v>92.9952510176391</v>
+        <v>94.1981390257252</v>
       </c>
       <c r="F194" t="n">
         <v>0</v>
@@ -6630,7 +6630,7 @@
         <v>19</v>
       </c>
       <c r="E195" t="n">
-        <v>93.9959294436906</v>
+        <v>95.1833607006021</v>
       </c>
       <c r="F195" t="n">
         <v>0</v>
@@ -6662,7 +6662,7 @@
         <v>19</v>
       </c>
       <c r="E196" t="n">
-        <v>96.9810040705563</v>
+        <v>96.9896004378763</v>
       </c>
       <c r="F196" t="n">
         <v>0</v>
@@ -6694,7 +6694,7 @@
         <v>19</v>
       </c>
       <c r="E197" t="n">
-        <v>100</v>
+        <v>97.4822112753147</v>
       </c>
       <c r="F197" t="n">
         <v>0</v>
@@ -6758,7 +6758,7 @@
         <v>19</v>
       </c>
       <c r="E199" t="n">
-        <v>29.0849673202614</v>
+        <v>30.0678221552374</v>
       </c>
       <c r="F199" t="n">
         <v>0</v>
@@ -6790,7 +6790,7 @@
         <v>19</v>
       </c>
       <c r="E200" t="n">
-        <v>76.1801016702977</v>
+        <v>66.46571213263</v>
       </c>
       <c r="F200" t="n">
         <v>0</v>
@@ -6822,7 +6822,7 @@
         <v>19</v>
       </c>
       <c r="E201" t="n">
-        <v>90.7770515613653</v>
+        <v>87.3398643556895</v>
       </c>
       <c r="F201" t="n">
         <v>0</v>
@@ -6854,7 +6854,7 @@
         <v>19</v>
       </c>
       <c r="E202" t="n">
-        <v>91.3943355119826</v>
+        <v>88.2441597588546</v>
       </c>
       <c r="F202" t="n">
         <v>0</v>
@@ -6886,7 +6886,7 @@
         <v>19</v>
       </c>
       <c r="E203" t="n">
-        <v>97.9665940450254</v>
+        <v>88.5455915599096</v>
       </c>
       <c r="F203" t="n">
         <v>0</v>
@@ -6918,7 +6918,7 @@
         <v>19</v>
       </c>
       <c r="E204" t="n">
-        <v>100</v>
+        <v>94.9510173323286</v>
       </c>
       <c r="F204" t="n">
         <v>0</v>
@@ -6982,7 +6982,7 @@
         <v>19</v>
       </c>
       <c r="E206" t="n">
-        <v>19.9664429530201</v>
+        <v>27.7358490566038</v>
       </c>
       <c r="F206" t="n">
         <v>0</v>
@@ -7014,7 +7014,7 @@
         <v>19</v>
       </c>
       <c r="E207" t="n">
-        <v>80.8724832214765</v>
+        <v>70.9905660377358</v>
       </c>
       <c r="F207" t="n">
         <v>0</v>
@@ -7046,7 +7046,7 @@
         <v>19</v>
       </c>
       <c r="E208" t="n">
-        <v>91.5268456375839</v>
+        <v>82.5943396226415</v>
       </c>
       <c r="F208" t="n">
         <v>0</v>
@@ -7078,7 +7078,7 @@
         <v>19</v>
       </c>
       <c r="E209" t="n">
-        <v>91.988255033557</v>
+        <v>85.377358490566</v>
       </c>
       <c r="F209" t="n">
         <v>0</v>
@@ -7110,7 +7110,7 @@
         <v>19</v>
       </c>
       <c r="E210" t="n">
-        <v>96.9798657718121</v>
+        <v>97.3584905660377</v>
       </c>
       <c r="F210" t="n">
         <v>0</v>
@@ -7142,7 +7142,7 @@
         <v>19</v>
       </c>
       <c r="E211" t="n">
-        <v>100</v>
+        <v>98.8679245283019</v>
       </c>
       <c r="F211" t="n">
         <v>0</v>
@@ -7206,7 +7206,7 @@
         <v>20</v>
       </c>
       <c r="E213" t="n">
-        <v>18.4673366834171</v>
+        <v>10.1608806096528</v>
       </c>
       <c r="F213" t="n">
         <v>1</v>
@@ -7238,7 +7238,7 @@
         <v>20</v>
       </c>
       <c r="E214" t="n">
-        <v>95.3517587939699</v>
+        <v>15.8340389500423</v>
       </c>
       <c r="F214" t="n">
         <v>1</v>
@@ -7270,7 +7270,7 @@
         <v>20</v>
       </c>
       <c r="E215" t="n">
-        <v>97.2361809045226</v>
+        <v>96.8670618120237</v>
       </c>
       <c r="F215" t="n">
         <v>1</v>
@@ -7302,7 +7302,7 @@
         <v>20</v>
       </c>
       <c r="E216" t="n">
-        <v>98.2412060301507</v>
+        <v>97.6291278577477</v>
       </c>
       <c r="F216" t="n">
         <v>1</v>
@@ -7334,7 +7334,7 @@
         <v>20</v>
       </c>
       <c r="E217" t="n">
-        <v>100</v>
+        <v>98.1371718882303</v>
       </c>
       <c r="F217" t="n">
         <v>1</v>
@@ -7430,7 +7430,7 @@
         <v>20</v>
       </c>
       <c r="E220" t="n">
-        <v>18.3948863636364</v>
+        <v>21.280276816609</v>
       </c>
       <c r="F220" t="n">
         <v>1</v>
@@ -7462,7 +7462,7 @@
         <v>20</v>
       </c>
       <c r="E221" t="n">
-        <v>50.7102272727273</v>
+        <v>65.3979238754325</v>
       </c>
       <c r="F221" t="n">
         <v>1</v>
@@ -7494,7 +7494,7 @@
         <v>20</v>
       </c>
       <c r="E222" t="n">
-        <v>66.9744318181818</v>
+        <v>84.6020761245675</v>
       </c>
       <c r="F222" t="n">
         <v>1</v>
@@ -7526,7 +7526,7 @@
         <v>20</v>
       </c>
       <c r="E223" t="n">
-        <v>84.4460227272727</v>
+        <v>90.8304498269896</v>
       </c>
       <c r="F223" t="n">
         <v>1</v>
@@ -7558,7 +7558,7 @@
         <v>20</v>
       </c>
       <c r="E224" t="n">
-        <v>92.8267045454545</v>
+        <v>99.1349480968858</v>
       </c>
       <c r="F224" t="n">
         <v>1</v>
@@ -7590,7 +7590,7 @@
         <v>20</v>
       </c>
       <c r="E225" t="n">
-        <v>97.0880681818182</v>
+        <v>100</v>
       </c>
       <c r="F225" t="n">
         <v>1</v>
@@ -7654,7 +7654,7 @@
         <v>20</v>
       </c>
       <c r="E227" t="n">
-        <v>17.9271708683473</v>
+        <v>1.88679245283019</v>
       </c>
       <c r="F227" t="n">
         <v>1</v>
@@ -7686,7 +7686,7 @@
         <v>20</v>
       </c>
       <c r="E228" t="n">
-        <v>22.4789915966387</v>
+        <v>2.35849056603774</v>
       </c>
       <c r="F228" t="n">
         <v>1</v>
@@ -7718,7 +7718,7 @@
         <v>20</v>
       </c>
       <c r="E229" t="n">
-        <v>56.3725490196078</v>
+        <v>6.44654088050314</v>
       </c>
       <c r="F229" t="n">
         <v>1</v>
@@ -7750,7 +7750,7 @@
         <v>20</v>
       </c>
       <c r="E230" t="n">
-        <v>87.4649859943978</v>
+        <v>47.6415094339623</v>
       </c>
       <c r="F230" t="n">
         <v>1</v>
@@ -7782,7 +7782,7 @@
         <v>20</v>
       </c>
       <c r="E231" t="n">
-        <v>92.5070028011204</v>
+        <v>74.3710691823899</v>
       </c>
       <c r="F231" t="n">
         <v>1</v>
@@ -7814,7 +7814,7 @@
         <v>20</v>
       </c>
       <c r="E232" t="n">
-        <v>94.2577030812325</v>
+        <v>86.7924528301887</v>
       </c>
       <c r="F232" t="n">
         <v>1</v>
@@ -7878,7 +7878,7 @@
         <v>20</v>
       </c>
       <c r="E234" t="n">
-        <v>13.9621240252506</v>
+        <v>2.02966432474629</v>
       </c>
       <c r="F234" t="n">
         <v>0</v>
@@ -7910,7 +7910,7 @@
         <v>20</v>
       </c>
       <c r="E235" t="n">
-        <v>17.5269216487189</v>
+        <v>3.94223263075722</v>
       </c>
       <c r="F235" t="n">
         <v>0</v>
@@ -7942,7 +7942,7 @@
         <v>20</v>
       </c>
       <c r="E236" t="n">
-        <v>50.2413665057557</v>
+        <v>9.21155347384856</v>
       </c>
       <c r="F236" t="n">
         <v>0</v>
@@ -7974,7 +7974,7 @@
         <v>20</v>
       </c>
       <c r="E237" t="n">
-        <v>80.9877460081693</v>
+        <v>12.8805620608899</v>
       </c>
       <c r="F237" t="n">
         <v>0</v>
@@ -8006,7 +8006,7 @@
         <v>20</v>
       </c>
       <c r="E238" t="n">
-        <v>94.0215373189751</v>
+        <v>30.9914129586261</v>
       </c>
       <c r="F238" t="n">
         <v>0</v>
@@ -8038,7 +8038,7 @@
         <v>20</v>
       </c>
       <c r="E239" t="n">
-        <v>99.814333457111</v>
+        <v>43.6377829820453</v>
       </c>
       <c r="F239" t="n">
         <v>0</v>
@@ -8102,7 +8102,7 @@
         <v>20</v>
       </c>
       <c r="E241" t="n">
-        <v>21.1764705882353</v>
+        <v>13.9733840304183</v>
       </c>
       <c r="F241" t="n">
         <v>0</v>
@@ -8134,7 +8134,7 @@
         <v>20</v>
       </c>
       <c r="E242" t="n">
-        <v>39.9396681749623</v>
+        <v>24.287072243346</v>
       </c>
       <c r="F242" t="n">
         <v>0</v>
@@ -8166,7 +8166,7 @@
         <v>20</v>
       </c>
       <c r="E243" t="n">
-        <v>48.6877828054299</v>
+        <v>51.3783269961977</v>
       </c>
       <c r="F243" t="n">
         <v>0</v>
@@ -8198,7 +8198,7 @@
         <v>20</v>
       </c>
       <c r="E244" t="n">
-        <v>61.6892911010558</v>
+        <v>78.754752851711</v>
       </c>
       <c r="F244" t="n">
         <v>0</v>
@@ -8230,7 +8230,7 @@
         <v>20</v>
       </c>
       <c r="E245" t="n">
-        <v>81.3876319758673</v>
+        <v>88.3555133079848</v>
       </c>
       <c r="F245" t="n">
         <v>0</v>
@@ -8262,7 +8262,7 @@
         <v>20</v>
       </c>
       <c r="E246" t="n">
-        <v>91.1010558069382</v>
+        <v>94.9619771863118</v>
       </c>
       <c r="F246" t="n">
         <v>0</v>
@@ -8326,7 +8326,7 @@
         <v>20</v>
       </c>
       <c r="E248" t="n">
-        <v>23.8774055595153</v>
+        <v>7.54300838112042</v>
       </c>
       <c r="F248" t="n">
         <v>0</v>
@@ -8358,7 +8358,7 @@
         <v>20</v>
       </c>
       <c r="E249" t="n">
-        <v>70.6343549536707</v>
+        <v>24.0405822673136</v>
       </c>
       <c r="F249" t="n">
         <v>0</v>
@@ -8390,7 +8390,7 @@
         <v>20</v>
       </c>
       <c r="E250" t="n">
-        <v>93.5495367070563</v>
+        <v>39.5677106307896</v>
       </c>
       <c r="F250" t="n">
         <v>0</v>
@@ -8422,7 +8422,7 @@
         <v>20</v>
       </c>
       <c r="E251" t="n">
-        <v>99.1446899501069</v>
+        <v>66.2990736656374</v>
       </c>
       <c r="F251" t="n">
         <v>0</v>
@@ -8454,7 +8454,7 @@
         <v>20</v>
       </c>
       <c r="E252" t="n">
-        <v>99.1446899501069</v>
+        <v>83.5465372739303</v>
       </c>
       <c r="F252" t="n">
         <v>0</v>
@@ -8486,7 +8486,7 @@
         <v>20</v>
       </c>
       <c r="E253" t="n">
-        <v>100</v>
+        <v>87.5606528451698</v>
       </c>
       <c r="F253" t="n">
         <v>0</v>
@@ -8550,7 +8550,7 @@
         <v>20</v>
       </c>
       <c r="E255" t="n">
-        <v>18.5126582278481</v>
+        <v>23.4901568234902</v>
       </c>
       <c r="F255" t="n">
         <v>0</v>
@@ -8582,7 +8582,7 @@
         <v>20</v>
       </c>
       <c r="E256" t="n">
-        <v>65.0316455696203</v>
+        <v>76.4097430764097</v>
       </c>
       <c r="F256" t="n">
         <v>0</v>
@@ -8614,7 +8614,7 @@
         <v>20</v>
       </c>
       <c r="E257" t="n">
-        <v>80.2215189873418</v>
+        <v>76.4097430764097</v>
       </c>
       <c r="F257" t="n">
         <v>0</v>
@@ -8646,7 +8646,7 @@
         <v>20</v>
       </c>
       <c r="E258" t="n">
-        <v>84.1772151898734</v>
+        <v>78.2782782782783</v>
       </c>
       <c r="F258" t="n">
         <v>0</v>
@@ -8678,7 +8678,7 @@
         <v>20</v>
       </c>
       <c r="E259" t="n">
-        <v>97.1518987341772</v>
+        <v>82.6493159826493</v>
       </c>
       <c r="F259" t="n">
         <v>0</v>
@@ -8710,7 +8710,7 @@
         <v>20</v>
       </c>
       <c r="E260" t="n">
-        <v>100</v>
+        <v>91.5248581915249</v>
       </c>
       <c r="F260" t="n">
         <v>0</v>
@@ -8774,7 +8774,7 @@
         <v>20</v>
       </c>
       <c r="E262" t="n">
-        <v>21.9638242894057</v>
+        <v>15.8113730929265</v>
       </c>
       <c r="F262" t="n">
         <v>0</v>
@@ -8806,7 +8806,7 @@
         <v>20</v>
       </c>
       <c r="E263" t="n">
-        <v>80.275624461671</v>
+        <v>75.1733703190014</v>
       </c>
       <c r="F263" t="n">
         <v>0</v>
@@ -8838,7 +8838,7 @@
         <v>20</v>
       </c>
       <c r="E264" t="n">
-        <v>88.8027562446167</v>
+        <v>76.005547850208</v>
       </c>
       <c r="F264" t="n">
         <v>0</v>
@@ -8870,7 +8870,7 @@
         <v>20</v>
       </c>
       <c r="E265" t="n">
-        <v>92.2480620155039</v>
+        <v>87.6560332871013</v>
       </c>
       <c r="F265" t="n">
         <v>0</v>
@@ -8902,7 +8902,7 @@
         <v>20</v>
       </c>
       <c r="E266" t="n">
-        <v>92.4203273040482</v>
+        <v>96.25520110957</v>
       </c>
       <c r="F266" t="n">
         <v>0</v>
@@ -8934,7 +8934,7 @@
         <v>20</v>
       </c>
       <c r="E267" t="n">
-        <v>96.9853574504737</v>
+        <v>100</v>
       </c>
       <c r="F267" t="n">
         <v>0</v>
@@ -8998,7 +8998,7 @@
         <v>20</v>
       </c>
       <c r="E269" t="n">
-        <v>27.2641509433962</v>
+        <v>30.2517850432168</v>
       </c>
       <c r="F269" t="n">
         <v>0</v>
@@ -9030,7 +9030,7 @@
         <v>20</v>
       </c>
       <c r="E270" t="n">
-        <v>61.9811320754717</v>
+        <v>80.9470124013529</v>
       </c>
       <c r="F270" t="n">
         <v>0</v>
@@ -9062,7 +9062,7 @@
         <v>20</v>
       </c>
       <c r="E271" t="n">
-        <v>75.8490566037736</v>
+        <v>90.717775272454</v>
       </c>
       <c r="F271" t="n">
         <v>0</v>
@@ -9094,7 +9094,7 @@
         <v>20</v>
       </c>
       <c r="E272" t="n">
-        <v>87.8301886792453</v>
+        <v>93.2732055618189</v>
       </c>
       <c r="F272" t="n">
         <v>0</v>
@@ -9126,7 +9126,7 @@
         <v>20</v>
       </c>
       <c r="E273" t="n">
-        <v>89.2452830188679</v>
+        <v>93.3859451334085</v>
       </c>
       <c r="F273" t="n">
         <v>0</v>
@@ -9158,7 +9158,7 @@
         <v>20</v>
       </c>
       <c r="E274" t="n">
-        <v>95</v>
+        <v>94.7763998496806</v>
       </c>
       <c r="F274" t="n">
         <v>0</v>
@@ -9222,7 +9222,7 @@
         <v>20</v>
       </c>
       <c r="E276" t="n">
-        <v>14.7960415158098</v>
+        <v>18.3967112024666</v>
       </c>
       <c r="F276" t="n">
         <v>0</v>
@@ -9254,7 +9254,7 @@
         <v>20</v>
       </c>
       <c r="E277" t="n">
-        <v>34.2988172821627</v>
+        <v>71.4285714285714</v>
       </c>
       <c r="F277" t="n">
         <v>0</v>
@@ -9286,7 +9286,7 @@
         <v>20</v>
       </c>
       <c r="E278" t="n">
-        <v>61.0909968621772</v>
+        <v>81.7574511819116</v>
       </c>
       <c r="F278" t="n">
         <v>0</v>
@@ -9318,7 +9318,7 @@
         <v>20</v>
       </c>
       <c r="E279" t="n">
-        <v>75.8387641805455</v>
+        <v>91.2127440904419</v>
       </c>
       <c r="F279" t="n">
         <v>0</v>
@@ -9350,7 +9350,7 @@
         <v>20</v>
       </c>
       <c r="E280" t="n">
-        <v>83.2971276852522</v>
+        <v>100</v>
       </c>
       <c r="F280" t="n">
         <v>0</v>
@@ -9382,7 +9382,7 @@
         <v>20</v>
       </c>
       <c r="E281" t="n">
-        <v>92.3244026068067</v>
+        <v>100</v>
       </c>
       <c r="F281" t="n">
         <v>0</v>
@@ -9446,7 +9446,7 @@
         <v>20</v>
       </c>
       <c r="E283" t="n">
-        <v>15.0060753341434</v>
+        <v>12.8468033775633</v>
       </c>
       <c r="F283" t="n">
         <v>0</v>
@@ -9478,7 +9478,7 @@
         <v>20</v>
       </c>
       <c r="E284" t="n">
-        <v>40.1883353584447</v>
+        <v>21.2002412545235</v>
       </c>
       <c r="F284" t="n">
         <v>0</v>
@@ -9510,7 +9510,7 @@
         <v>20</v>
       </c>
       <c r="E285" t="n">
-        <v>79.9817739975699</v>
+        <v>61.7913148371532</v>
       </c>
       <c r="F285" t="n">
         <v>0</v>
@@ -9542,7 +9542,7 @@
         <v>20</v>
       </c>
       <c r="E286" t="n">
-        <v>82.0777642770352</v>
+        <v>82.4788902291918</v>
       </c>
       <c r="F286" t="n">
         <v>0</v>
@@ -9574,7 +9574,7 @@
         <v>20</v>
       </c>
       <c r="E287" t="n">
-        <v>84.6294046172539</v>
+        <v>88.8721351025332</v>
       </c>
       <c r="F287" t="n">
         <v>0</v>
@@ -9606,7 +9606,7 @@
         <v>20</v>
       </c>
       <c r="E288" t="n">
-        <v>91.9805589307412</v>
+        <v>91.8878166465621</v>
       </c>
       <c r="F288" t="n">
         <v>0</v>
@@ -9670,7 +9670,7 @@
         <v>20</v>
       </c>
       <c r="E290" t="n">
-        <v>4.09988818486769</v>
+        <v>19.3863939528679</v>
       </c>
       <c r="F290" t="n">
         <v>0</v>
@@ -9702,7 +9702,7 @@
         <v>20</v>
       </c>
       <c r="E291" t="n">
-        <v>13.2687290346627</v>
+        <v>52.9568697198755</v>
       </c>
       <c r="F291" t="n">
         <v>0</v>
@@ -9734,7 +9734,7 @@
         <v>20</v>
       </c>
       <c r="E292" t="n">
-        <v>42.9370108087961</v>
+        <v>67.718986216096</v>
       </c>
       <c r="F292" t="n">
         <v>0</v>
@@ -9766,7 +9766,7 @@
         <v>20</v>
       </c>
       <c r="E293" t="n">
-        <v>59.7838240775252</v>
+        <v>77.0120053357048</v>
       </c>
       <c r="F293" t="n">
         <v>0</v>
@@ -9798,7 +9798,7 @@
         <v>20</v>
       </c>
       <c r="E294" t="n">
-        <v>72.8289228475587</v>
+        <v>84.9710982658959</v>
       </c>
       <c r="F294" t="n">
         <v>0</v>
@@ -9830,7 +9830,7 @@
         <v>20</v>
       </c>
       <c r="E295" t="n">
-        <v>86.1349235929929</v>
+        <v>89.3730546909738</v>
       </c>
       <c r="F295" t="n">
         <v>0</v>
@@ -9894,7 +9894,7 @@
         <v>20</v>
       </c>
       <c r="E297" t="n">
-        <v>40.2679568291775</v>
+        <v>25.1535455053043</v>
       </c>
       <c r="F297" t="n">
         <v>0</v>
@@ -9926,7 +9926,7 @@
         <v>20</v>
       </c>
       <c r="E298" t="n">
-        <v>82.8433196873837</v>
+        <v>89.5030709101061</v>
       </c>
       <c r="F298" t="n">
         <v>0</v>
@@ -9958,7 +9958,7 @@
         <v>20</v>
       </c>
       <c r="E299" t="n">
-        <v>93.9337551172311</v>
+        <v>94.2769402568398</v>
       </c>
       <c r="F299" t="n">
         <v>0</v>
@@ -9990,7 +9990,7 @@
         <v>20</v>
       </c>
       <c r="E300" t="n">
-        <v>94.3431336062523</v>
+        <v>95.9240647682859</v>
       </c>
       <c r="F300" t="n">
         <v>0</v>
@@ -10022,7 +10022,7 @@
         <v>20</v>
       </c>
       <c r="E301" t="n">
-        <v>97.9903237811686</v>
+        <v>96.3149078726968</v>
       </c>
       <c r="F301" t="n">
         <v>0</v>
@@ -10054,7 +10054,7 @@
         <v>20</v>
       </c>
       <c r="E302" t="n">
-        <v>100</v>
+        <v>97.319932998325</v>
       </c>
       <c r="F302" t="n">
         <v>0</v>
@@ -10118,7 +10118,7 @@
         <v>20</v>
       </c>
       <c r="E304" t="n">
-        <v>29.3115942028986</v>
+        <v>30.2207130730051</v>
       </c>
       <c r="F304" t="n">
         <v>0</v>
@@ -10150,7 +10150,7 @@
         <v>20</v>
       </c>
       <c r="E305" t="n">
-        <v>74.7826086956522</v>
+        <v>65.365025466893</v>
       </c>
       <c r="F305" t="n">
         <v>0</v>
@@ -10182,7 +10182,7 @@
         <v>20</v>
       </c>
       <c r="E306" t="n">
-        <v>91.9565217391304</v>
+        <v>89.6434634974533</v>
       </c>
       <c r="F306" t="n">
         <v>0</v>
@@ -10214,7 +10214,7 @@
         <v>20</v>
       </c>
       <c r="E307" t="n">
-        <v>92.463768115942</v>
+        <v>90.0679117147708</v>
       </c>
       <c r="F307" t="n">
         <v>0</v>
@@ -10246,7 +10246,7 @@
         <v>20</v>
       </c>
       <c r="E308" t="n">
-        <v>96.268115942029</v>
+        <v>91.0016977928693</v>
       </c>
       <c r="F308" t="n">
         <v>0</v>
@@ -10278,7 +10278,7 @@
         <v>20</v>
       </c>
       <c r="E309" t="n">
-        <v>100</v>
+        <v>95.3310696095076</v>
       </c>
       <c r="F309" t="n">
         <v>0</v>
@@ -10342,7 +10342,7 @@
         <v>20</v>
       </c>
       <c r="E311" t="n">
-        <v>18.1034482758621</v>
+        <v>29.6761720637989</v>
       </c>
       <c r="F311" t="n">
         <v>0</v>
@@ -10374,7 +10374,7 @@
         <v>20</v>
       </c>
       <c r="E312" t="n">
-        <v>78.8362068965517</v>
+        <v>68.9705171580474</v>
       </c>
       <c r="F312" t="n">
         <v>0</v>
@@ -10406,7 +10406,7 @@
         <v>20</v>
       </c>
       <c r="E313" t="n">
-        <v>91.9827586206897</v>
+        <v>82.5036249395843</v>
       </c>
       <c r="F313" t="n">
         <v>0</v>
@@ -10438,7 +10438,7 @@
         <v>20</v>
       </c>
       <c r="E314" t="n">
-        <v>92.3706896551724</v>
+        <v>93.7167713871436</v>
       </c>
       <c r="F314" t="n">
         <v>0</v>
@@ -10470,7 +10470,7 @@
         <v>20</v>
       </c>
       <c r="E315" t="n">
-        <v>98.2758620689655</v>
+        <v>96.4233929434509</v>
       </c>
       <c r="F315" t="n">
         <v>0</v>
@@ -10502,7 +10502,7 @@
         <v>20</v>
       </c>
       <c r="E316" t="n">
-        <v>100</v>
+        <v>98.9850169163847</v>
       </c>
       <c r="F316" t="n">
         <v>0</v>
@@ -20738,7 +20738,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="n">
-        <v>8.9943342776204</v>
+        <v>18.2134570765661</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
@@ -20770,7 +20770,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>15.1558073654391</v>
+        <v>93.7354988399072</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -20802,7 +20802,7 @@
         <v>12</v>
       </c>
       <c r="E5" t="n">
-        <v>93.7677053824363</v>
+        <v>94.8955916473318</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
@@ -20834,7 +20834,7 @@
         <v>12</v>
       </c>
       <c r="E6" t="n">
-        <v>94.3342776203966</v>
+        <v>97.7958236658933</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
@@ -20866,7 +20866,7 @@
         <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>95.042492917847</v>
+        <v>100</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -20962,7 +20962,7 @@
         <v>12</v>
       </c>
       <c r="E10" t="n">
-        <v>21.583850931677</v>
+        <v>18.2192910140148</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -20994,7 +20994,7 @@
         <v>12</v>
       </c>
       <c r="E11" t="n">
-        <v>66.6149068322981</v>
+        <v>45.6718878812861</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
@@ -21026,7 +21026,7 @@
         <v>12</v>
       </c>
       <c r="E12" t="n">
-        <v>83.0745341614907</v>
+        <v>68.5902720527617</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
@@ -21058,7 +21058,7 @@
         <v>12</v>
       </c>
       <c r="E13" t="n">
-        <v>91.4596273291926</v>
+        <v>81.2860676009893</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -21090,7 +21090,7 @@
         <v>12</v>
       </c>
       <c r="E14" t="n">
-        <v>96.1180124223602</v>
+        <v>93.3223413025556</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -21186,7 +21186,7 @@
         <v>12</v>
       </c>
       <c r="E17" t="n">
-        <v>1.96850393700787</v>
+        <v>16.1073825503356</v>
       </c>
       <c r="F17" t="n">
         <v>1</v>
@@ -21218,7 +21218,7 @@
         <v>12</v>
       </c>
       <c r="E18" t="n">
-        <v>2.36220472440945</v>
+        <v>27.4651522973671</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
@@ -21250,7 +21250,7 @@
         <v>12</v>
       </c>
       <c r="E19" t="n">
-        <v>7.48031496062992</v>
+        <v>59.9380485286526</v>
       </c>
       <c r="F19" t="n">
         <v>1</v>
@@ -21282,7 +21282,7 @@
         <v>12</v>
       </c>
       <c r="E20" t="n">
-        <v>47.1128608923885</v>
+        <v>83.6344863190501</v>
       </c>
       <c r="F20" t="n">
         <v>1</v>
@@ -21314,7 +21314,7 @@
         <v>12</v>
       </c>
       <c r="E21" t="n">
-        <v>74.9343832020997</v>
+        <v>93.9597315436242</v>
       </c>
       <c r="F21" t="n">
         <v>1</v>
@@ -21346,7 +21346,7 @@
         <v>12</v>
       </c>
       <c r="E22" t="n">
-        <v>86.8766404199475</v>
+        <v>97.9349509550852</v>
       </c>
       <c r="F22" t="n">
         <v>1</v>
@@ -21410,7 +21410,7 @@
         <v>12</v>
       </c>
       <c r="E24" t="n">
-        <v>2.5944469731452</v>
+        <v>14.9615851192883</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -21442,7 +21442,7 @@
         <v>12</v>
       </c>
       <c r="E25" t="n">
-        <v>3.95994538006372</v>
+        <v>19.3691872219976</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -21474,7 +21474,7 @@
         <v>12</v>
       </c>
       <c r="E26" t="n">
-        <v>8.19299044151115</v>
+        <v>47.4727052163364</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -21506,7 +21506,7 @@
         <v>12</v>
       </c>
       <c r="E27" t="n">
-        <v>13.882567137005</v>
+        <v>82.9761423372422</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -21538,7 +21538,7 @@
         <v>12</v>
       </c>
       <c r="E28" t="n">
-        <v>30.7692307692308</v>
+        <v>89.7290739991913</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -21570,7 +21570,7 @@
         <v>12</v>
       </c>
       <c r="E29" t="n">
-        <v>43.468365953573</v>
+        <v>97.9781641730691</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -21634,7 +21634,7 @@
         <v>12</v>
       </c>
       <c r="E31" t="n">
-        <v>14.931650893796</v>
+        <v>19.817439346625</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -21666,7 +21666,7 @@
         <v>12</v>
       </c>
       <c r="E32" t="n">
-        <v>23.5541535226078</v>
+        <v>39.8750900792698</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -21698,7 +21698,7 @@
         <v>12</v>
       </c>
       <c r="E33" t="n">
-        <v>50.9989484752892</v>
+        <v>59.0439586836416</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -21730,7 +21730,7 @@
         <v>12</v>
       </c>
       <c r="E34" t="n">
-        <v>78.7066246056782</v>
+        <v>70.9344222916166</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -21762,7 +21762,7 @@
         <v>12</v>
       </c>
       <c r="E35" t="n">
-        <v>87.0662460567823</v>
+        <v>84.914724957963</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -21794,7 +21794,7 @@
         <v>12</v>
       </c>
       <c r="E36" t="n">
-        <v>96.267087276551</v>
+        <v>94.0427576267115</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -21858,7 +21858,7 @@
         <v>12</v>
       </c>
       <c r="E38" t="n">
-        <v>8.38654746700724</v>
+        <v>19.9732501114579</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -21890,7 +21890,7 @@
         <v>12</v>
       </c>
       <c r="E39" t="n">
-        <v>22.3925074499787</v>
+        <v>62.9959875167187</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
@@ -21922,7 +21922,7 @@
         <v>12</v>
       </c>
       <c r="E40" t="n">
-        <v>41.8901660280971</v>
+        <v>97.9045920641997</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -21954,7 +21954,7 @@
         <v>12</v>
       </c>
       <c r="E41" t="n">
-        <v>65.6875266070668</v>
+        <v>98.4841729826126</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -21986,7 +21986,7 @@
         <v>12</v>
       </c>
       <c r="E42" t="n">
-        <v>83.1843337590464</v>
+        <v>98.4841729826126</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -22018,7 +22018,7 @@
         <v>12</v>
       </c>
       <c r="E43" t="n">
-        <v>86.6751809280545</v>
+        <v>100</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -22082,7 +22082,7 @@
         <v>12</v>
       </c>
       <c r="E45" t="n">
-        <v>22.972972972973</v>
+        <v>23.9520958083832</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -22114,7 +22114,7 @@
         <v>12</v>
       </c>
       <c r="E46" t="n">
-        <v>74.0753911806543</v>
+        <v>65.9680638722555</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -22146,7 +22146,7 @@
         <v>12</v>
       </c>
       <c r="E47" t="n">
-        <v>74.0753911806543</v>
+        <v>82.5349301397206</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -22178,7 +22178,7 @@
         <v>12</v>
       </c>
       <c r="E48" t="n">
-        <v>77.4893314366999</v>
+        <v>89.6207584830339</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -22210,7 +22210,7 @@
         <v>12</v>
       </c>
       <c r="E49" t="n">
-        <v>81.9701280227596</v>
+        <v>96.0079840319361</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -22242,7 +22242,7 @@
         <v>12</v>
       </c>
       <c r="E50" t="n">
-        <v>90.9672830725462</v>
+        <v>100</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
@@ -22306,7 +22306,7 @@
         <v>12</v>
       </c>
       <c r="E52" t="n">
-        <v>14.2857142857143</v>
+        <v>19.971671388102</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -22338,7 +22338,7 @@
         <v>12</v>
       </c>
       <c r="E53" t="n">
-        <v>71.865889212828</v>
+        <v>79.1784702549575</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -22370,7 +22370,7 @@
         <v>12</v>
       </c>
       <c r="E54" t="n">
-        <v>75.5102040816327</v>
+        <v>88.9518413597734</v>
       </c>
       <c r="F54" t="n">
         <v>0</v>
@@ -22402,7 +22402,7 @@
         <v>12</v>
       </c>
       <c r="E55" t="n">
-        <v>87.4635568513119</v>
+        <v>91.8555240793201</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
@@ -22434,7 +22434,7 @@
         <v>12</v>
       </c>
       <c r="E56" t="n">
-        <v>94.6064139941691</v>
+        <v>94.0509915014164</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
@@ -22466,7 +22466,7 @@
         <v>12</v>
       </c>
       <c r="E57" t="n">
-        <v>100</v>
+        <v>98.0878186968839</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
@@ -22530,7 +22530,7 @@
         <v>12</v>
       </c>
       <c r="E59" t="n">
-        <v>29.5936395759717</v>
+        <v>26.26953125</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
@@ -22562,7 +22562,7 @@
         <v>12</v>
       </c>
       <c r="E60" t="n">
-        <v>80.9628975265018</v>
+        <v>59.375</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
@@ -22594,7 +22594,7 @@
         <v>12</v>
       </c>
       <c r="E61" t="n">
-        <v>89.2667844522968</v>
+        <v>76.953125</v>
       </c>
       <c r="F61" t="n">
         <v>0</v>
@@ -22626,7 +22626,7 @@
         <v>12</v>
       </c>
       <c r="E62" t="n">
-        <v>91.9611307420495</v>
+        <v>87.109375</v>
       </c>
       <c r="F62" t="n">
         <v>0</v>
@@ -22658,7 +22658,7 @@
         <v>12</v>
       </c>
       <c r="E63" t="n">
-        <v>92.2703180212014</v>
+        <v>88.96484375</v>
       </c>
       <c r="F63" t="n">
         <v>0</v>
@@ -22690,7 +22690,7 @@
         <v>12</v>
       </c>
       <c r="E64" t="n">
-        <v>96.1572438162544</v>
+        <v>95.60546875</v>
       </c>
       <c r="F64" t="n">
         <v>0</v>
@@ -22754,7 +22754,7 @@
         <v>12</v>
       </c>
       <c r="E66" t="n">
-        <v>17.8705440900563</v>
+        <v>13.7733142037303</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
@@ -22786,7 +22786,7 @@
         <v>12</v>
       </c>
       <c r="E67" t="n">
-        <v>71.6228893058161</v>
+        <v>29.9856527977045</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
@@ -22818,7 +22818,7 @@
         <v>12</v>
       </c>
       <c r="E68" t="n">
-        <v>79.9718574108818</v>
+        <v>58.4791965566715</v>
       </c>
       <c r="F68" t="n">
         <v>0</v>
@@ -22850,7 +22850,7 @@
         <v>12</v>
       </c>
       <c r="E69" t="n">
-        <v>91.1350844277674</v>
+        <v>77.3027259684362</v>
       </c>
       <c r="F69" t="n">
         <v>0</v>
@@ -22882,7 +22882,7 @@
         <v>12</v>
       </c>
       <c r="E70" t="n">
-        <v>100</v>
+        <v>82.5824964131994</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
@@ -22914,7 +22914,7 @@
         <v>12</v>
       </c>
       <c r="E71" t="n">
-        <v>100</v>
+        <v>93.4863701578192</v>
       </c>
       <c r="F71" t="n">
         <v>0</v>
@@ -22978,7 +22978,7 @@
         <v>12</v>
       </c>
       <c r="E73" t="n">
-        <v>13.5854341736695</v>
+        <v>15.9838817998657</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
@@ -23010,7 +23010,7 @@
         <v>12</v>
       </c>
       <c r="E74" t="n">
-        <v>21.6736694677871</v>
+        <v>38.9858965748825</v>
       </c>
       <c r="F74" t="n">
         <v>0</v>
@@ -23042,7 +23042,7 @@
         <v>12</v>
       </c>
       <c r="E75" t="n">
-        <v>59.9789915966387</v>
+        <v>77.2666218938885</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
@@ -23074,7 +23074,7 @@
         <v>12</v>
       </c>
       <c r="E76" t="n">
-        <v>83.9985994397759</v>
+        <v>85.0906648757555</v>
       </c>
       <c r="F76" t="n">
         <v>0</v>
@@ -23106,7 +23106,7 @@
         <v>12</v>
       </c>
       <c r="E77" t="n">
-        <v>87.3949579831933</v>
+        <v>86.7696440564137</v>
       </c>
       <c r="F77" t="n">
         <v>0</v>
@@ -23138,7 +23138,7 @@
         <v>12</v>
       </c>
       <c r="E78" t="n">
-        <v>93.8725490196078</v>
+        <v>90.1947615849564</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
@@ -23202,7 +23202,7 @@
         <v>12</v>
       </c>
       <c r="E80" t="n">
-        <v>19.9920979849862</v>
+        <v>2.40096038415366</v>
       </c>
       <c r="F80" t="n">
         <v>0</v>
@@ -23234,7 +23234,7 @@
         <v>12</v>
       </c>
       <c r="E81" t="n">
-        <v>53.0225207427894</v>
+        <v>10.484193677471</v>
       </c>
       <c r="F81" t="n">
         <v>0</v>
@@ -23266,7 +23266,7 @@
         <v>12</v>
       </c>
       <c r="E82" t="n">
-        <v>68.4709600948242</v>
+        <v>42.6570628251301</v>
       </c>
       <c r="F82" t="n">
         <v>0</v>
@@ -23298,7 +23298,7 @@
         <v>12</v>
       </c>
       <c r="E83" t="n">
-        <v>77.3607269853813</v>
+        <v>63.1852741096439</v>
       </c>
       <c r="F83" t="n">
         <v>0</v>
@@ -23330,7 +23330,7 @@
         <v>12</v>
       </c>
       <c r="E84" t="n">
-        <v>85.7368629000395</v>
+        <v>72.9891956782713</v>
       </c>
       <c r="F84" t="n">
         <v>0</v>
@@ -23362,7 +23362,7 @@
         <v>12</v>
       </c>
       <c r="E85" t="n">
-        <v>91.2682734097195</v>
+        <v>89.9959983993597</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -23426,7 +23426,7 @@
         <v>12</v>
       </c>
       <c r="E87" t="n">
-        <v>25.7982120051086</v>
+        <v>40.9867784585618</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -23458,7 +23458,7 @@
         <v>12</v>
       </c>
       <c r="E88" t="n">
-        <v>89.9744572158365</v>
+        <v>92.9861335053209</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -23490,7 +23490,7 @@
         <v>12</v>
       </c>
       <c r="E89" t="n">
-        <v>93.3908045977011</v>
+        <v>95.6626894550145</v>
       </c>
       <c r="F89" t="n">
         <v>0</v>
@@ -23522,7 +23522,7 @@
         <v>12</v>
       </c>
       <c r="E90" t="n">
-        <v>94.5721583652618</v>
+        <v>95.9045469203483</v>
       </c>
       <c r="F90" t="n">
         <v>0</v>
@@ -23554,7 +23554,7 @@
         <v>12</v>
       </c>
       <c r="E91" t="n">
-        <v>96.9987228607918</v>
+        <v>96.0980328926153</v>
       </c>
       <c r="F91" t="n">
         <v>0</v>
@@ -23586,7 +23586,7 @@
         <v>12</v>
       </c>
       <c r="E92" t="n">
-        <v>97.57343550447</v>
+        <v>100</v>
       </c>
       <c r="F92" t="n">
         <v>0</v>
@@ -23650,7 +23650,7 @@
         <v>12</v>
       </c>
       <c r="E94" t="n">
-        <v>30.5336832895888</v>
+        <v>27.9881217520416</v>
       </c>
       <c r="F94" t="n">
         <v>0</v>
@@ -23682,7 +23682,7 @@
         <v>12</v>
       </c>
       <c r="E95" t="n">
-        <v>65.4418197725284</v>
+        <v>73.5708982925019</v>
       </c>
       <c r="F95" t="n">
         <v>0</v>
@@ -23714,7 +23714,7 @@
         <v>12</v>
       </c>
       <c r="E96" t="n">
-        <v>87.5765529308837</v>
+        <v>90.9428359317001</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
@@ -23746,7 +23746,7 @@
         <v>12</v>
       </c>
       <c r="E97" t="n">
-        <v>88.1889763779528</v>
+        <v>91.5738678544915</v>
       </c>
       <c r="F97" t="n">
         <v>0</v>
@@ -23778,7 +23778,7 @@
         <v>12</v>
       </c>
       <c r="E98" t="n">
-        <v>88.9763779527559</v>
+        <v>96.9933184855234</v>
       </c>
       <c r="F98" t="n">
         <v>0</v>
@@ -23810,7 +23810,7 @@
         <v>12</v>
       </c>
       <c r="E99" t="n">
-        <v>94.925634295713</v>
+        <v>100</v>
       </c>
       <c r="F99" t="n">
         <v>0</v>
@@ -23874,7 +23874,7 @@
         <v>12</v>
       </c>
       <c r="E101" t="n">
-        <v>22.3482699943279</v>
+        <v>21.9858156028369</v>
       </c>
       <c r="F101" t="n">
         <v>0</v>
@@ -23906,7 +23906,7 @@
         <v>12</v>
       </c>
       <c r="E102" t="n">
-        <v>70.5615428247306</v>
+        <v>80.2748226950355</v>
       </c>
       <c r="F102" t="n">
         <v>0</v>
@@ -23938,7 +23938,7 @@
         <v>12</v>
       </c>
       <c r="E103" t="n">
-        <v>81.5655133295519</v>
+        <v>91.6666666666667</v>
       </c>
       <c r="F103" t="n">
         <v>0</v>
@@ -23970,7 +23970,7 @@
         <v>12</v>
       </c>
       <c r="E104" t="n">
-        <v>91.26488939308</v>
+        <v>92.9078014184397</v>
       </c>
       <c r="F104" t="n">
         <v>0</v>
@@ -24002,7 +24002,7 @@
         <v>12</v>
       </c>
       <c r="E105" t="n">
-        <v>96.483267158253</v>
+        <v>94.3262411347518</v>
       </c>
       <c r="F105" t="n">
         <v>0</v>
@@ -24034,7 +24034,7 @@
         <v>12</v>
       </c>
       <c r="E106" t="n">
-        <v>98.1281905842314</v>
+        <v>100</v>
       </c>
       <c r="F106" t="n">
         <v>0</v>
@@ -24098,7 +24098,7 @@
         <v>19</v>
       </c>
       <c r="E108" t="n">
-        <v>9.29626411815812</v>
+        <v>18.0115273775216</v>
       </c>
       <c r="F108" t="n">
         <v>1</v>
@@ -24130,7 +24130,7 @@
         <v>19</v>
       </c>
       <c r="E109" t="n">
-        <v>15.2041702867072</v>
+        <v>92.3631123919308</v>
       </c>
       <c r="F109" t="n">
         <v>1</v>
@@ -24162,7 +24162,7 @@
         <v>19</v>
       </c>
       <c r="E110" t="n">
-        <v>94.1789748045178</v>
+        <v>95.6772334293948</v>
       </c>
       <c r="F110" t="n">
         <v>1</v>
@@ -24194,7 +24194,7 @@
         <v>19</v>
       </c>
       <c r="E111" t="n">
-        <v>94.7871416159861</v>
+        <v>97.8386167146974</v>
       </c>
       <c r="F111" t="n">
         <v>1</v>
@@ -24226,7 +24226,7 @@
         <v>19</v>
       </c>
       <c r="E112" t="n">
-        <v>95.4821894005213</v>
+        <v>100</v>
       </c>
       <c r="F112" t="n">
         <v>1</v>
@@ -24322,7 +24322,7 @@
         <v>19</v>
       </c>
       <c r="E115" t="n">
-        <v>22.2591362126246</v>
+        <v>18.7126741871267</v>
       </c>
       <c r="F115" t="n">
         <v>1</v>
@@ -24354,7 +24354,7 @@
         <v>19</v>
       </c>
       <c r="E116" t="n">
-        <v>65.2823920265781</v>
+        <v>49.6350364963504</v>
       </c>
       <c r="F116" t="n">
         <v>1</v>
@@ -24386,7 +24386,7 @@
         <v>19</v>
       </c>
       <c r="E117" t="n">
-        <v>85.0498338870432</v>
+        <v>66.9542136695421</v>
       </c>
       <c r="F117" t="n">
         <v>1</v>
@@ -24418,7 +24418,7 @@
         <v>19</v>
       </c>
       <c r="E118" t="n">
-        <v>90.0332225913621</v>
+        <v>81.8181818181818</v>
       </c>
       <c r="F118" t="n">
         <v>1</v>
@@ -24450,7 +24450,7 @@
         <v>19</v>
       </c>
       <c r="E119" t="n">
-        <v>97.0099667774086</v>
+        <v>92.9661579296616</v>
       </c>
       <c r="F119" t="n">
         <v>1</v>
@@ -24482,7 +24482,7 @@
         <v>19</v>
       </c>
       <c r="E120" t="n">
-        <v>100</v>
+        <v>99.535500995355</v>
       </c>
       <c r="F120" t="n">
         <v>1</v>
@@ -24546,7 +24546,7 @@
         <v>19</v>
       </c>
       <c r="E122" t="n">
-        <v>1.35135135135135</v>
+        <v>16.1499639509733</v>
       </c>
       <c r="F122" t="n">
         <v>1</v>
@@ -24578,7 +24578,7 @@
         <v>19</v>
       </c>
       <c r="E123" t="n">
-        <v>2.25225225225225</v>
+        <v>25.0180245133381</v>
       </c>
       <c r="F123" t="n">
         <v>1</v>
@@ -24610,7 +24610,7 @@
         <v>19</v>
       </c>
       <c r="E124" t="n">
-        <v>6.90690690690691</v>
+        <v>58.9762076423937</v>
       </c>
       <c r="F124" t="n">
         <v>1</v>
@@ -24642,7 +24642,7 @@
         <v>19</v>
       </c>
       <c r="E125" t="n">
-        <v>49.2492492492492</v>
+        <v>83.8500360490267</v>
       </c>
       <c r="F125" t="n">
         <v>1</v>
@@ -24674,7 +24674,7 @@
         <v>19</v>
       </c>
       <c r="E126" t="n">
-        <v>73.8738738738739</v>
+        <v>91.9250180245133</v>
       </c>
       <c r="F126" t="n">
         <v>1</v>
@@ -24706,7 +24706,7 @@
         <v>19</v>
       </c>
       <c r="E127" t="n">
-        <v>87.987987987988</v>
+        <v>96.6834895457823</v>
       </c>
       <c r="F127" t="n">
         <v>1</v>
@@ -24770,7 +24770,7 @@
         <v>19</v>
       </c>
       <c r="E129" t="n">
-        <v>2.00426439232409</v>
+        <v>15.0036954915004</v>
       </c>
       <c r="F129" t="n">
         <v>0</v>
@@ -24802,7 +24802,7 @@
         <v>19</v>
       </c>
       <c r="E130" t="n">
-        <v>4.26439232409382</v>
+        <v>18.0709534368071</v>
       </c>
       <c r="F130" t="n">
         <v>0</v>
@@ -24834,7 +24834,7 @@
         <v>19</v>
       </c>
       <c r="E131" t="n">
-        <v>8.86993603411514</v>
+        <v>52.069475240207</v>
       </c>
       <c r="F131" t="n">
         <v>0</v>
@@ -24866,7 +24866,7 @@
         <v>19</v>
       </c>
       <c r="E132" t="n">
-        <v>13.8592750533049</v>
+        <v>79.490022172949</v>
       </c>
       <c r="F132" t="n">
         <v>0</v>
@@ -24898,7 +24898,7 @@
         <v>19</v>
       </c>
       <c r="E133" t="n">
-        <v>31.4712153518124</v>
+        <v>90.5025868440503</v>
       </c>
       <c r="F133" t="n">
         <v>0</v>
@@ -24930,7 +24930,7 @@
         <v>19</v>
       </c>
       <c r="E134" t="n">
-        <v>45.6716417910448</v>
+        <v>94.9371766444937</v>
       </c>
       <c r="F134" t="n">
         <v>0</v>
@@ -24994,7 +24994,7 @@
         <v>19</v>
       </c>
       <c r="E136" t="n">
-        <v>13.376987839102</v>
+        <v>22.4066390041494</v>
       </c>
       <c r="F136" t="n">
         <v>0</v>
@@ -25026,7 +25026,7 @@
         <v>19</v>
       </c>
       <c r="E137" t="n">
-        <v>24.7427502338634</v>
+        <v>41.49377593361</v>
       </c>
       <c r="F137" t="n">
         <v>0</v>
@@ -25058,7 +25058,7 @@
         <v>19</v>
       </c>
       <c r="E138" t="n">
-        <v>50</v>
+        <v>54.1078838174274</v>
       </c>
       <c r="F138" t="n">
         <v>0</v>
@@ -25090,7 +25090,7 @@
         <v>19</v>
       </c>
       <c r="E139" t="n">
-        <v>80.355472404116</v>
+        <v>65.9751037344398</v>
       </c>
       <c r="F139" t="n">
         <v>0</v>
@@ -25122,7 +25122,7 @@
         <v>19</v>
       </c>
       <c r="E140" t="n">
-        <v>89.289055191768</v>
+        <v>91.9087136929461</v>
       </c>
       <c r="F140" t="n">
         <v>0</v>
@@ -25154,7 +25154,7 @@
         <v>19</v>
       </c>
       <c r="E141" t="n">
-        <v>95.3695042095416</v>
+        <v>89.9170124481328</v>
       </c>
       <c r="F141" t="n">
         <v>0</v>
@@ -25218,7 +25218,7 @@
         <v>19</v>
       </c>
       <c r="E143" t="n">
-        <v>7.87781350482315</v>
+        <v>28.0328480776409</v>
       </c>
       <c r="F143" t="n">
         <v>0</v>
@@ -25250,7 +25250,7 @@
         <v>19</v>
       </c>
       <c r="E144" t="n">
-        <v>23.9951768488746</v>
+        <v>64.9869354236655</v>
       </c>
       <c r="F144" t="n">
         <v>0</v>
@@ -25282,7 +25282,7 @@
         <v>19</v>
       </c>
       <c r="E145" t="n">
-        <v>41.5996784565916</v>
+        <v>95.9686450167973</v>
       </c>
       <c r="F145" t="n">
         <v>0</v>
@@ -25314,7 +25314,7 @@
         <v>19</v>
       </c>
       <c r="E146" t="n">
-        <v>66.7604501607717</v>
+        <v>96.7898469578201</v>
       </c>
       <c r="F146" t="n">
         <v>0</v>
@@ -25346,7 +25346,7 @@
         <v>19</v>
       </c>
       <c r="E147" t="n">
-        <v>84.5659163987138</v>
+        <v>96.7898469578201</v>
       </c>
       <c r="F147" t="n">
         <v>0</v>
@@ -25378,7 +25378,7 @@
         <v>19</v>
       </c>
       <c r="E148" t="n">
-        <v>86.2942122186495</v>
+        <v>100</v>
       </c>
       <c r="F148" t="n">
         <v>0</v>
@@ -25442,7 +25442,7 @@
         <v>19</v>
       </c>
       <c r="E150" t="n">
-        <v>22.3765996343693</v>
+        <v>21.9165085388994</v>
       </c>
       <c r="F150" t="n">
         <v>0</v>
@@ -25474,7 +25474,7 @@
         <v>19</v>
       </c>
       <c r="E151" t="n">
-        <v>75.2833638025594</v>
+        <v>66.7931688804554</v>
       </c>
       <c r="F151" t="n">
         <v>0</v>
@@ -25506,7 +25506,7 @@
         <v>19</v>
       </c>
       <c r="E152" t="n">
-        <v>75.2833638025594</v>
+        <v>82.9222011385199</v>
       </c>
       <c r="F152" t="n">
         <v>0</v>
@@ -25538,7 +25538,7 @@
         <v>19</v>
       </c>
       <c r="E153" t="n">
-        <v>78.2815356489945</v>
+        <v>87.4762808349146</v>
       </c>
       <c r="F153" t="n">
         <v>0</v>
@@ -25570,7 +25570,7 @@
         <v>19</v>
       </c>
       <c r="E154" t="n">
-        <v>81.3893967093236</v>
+        <v>91.8406072106262</v>
       </c>
       <c r="F154" t="n">
         <v>0</v>
@@ -25602,7 +25602,7 @@
         <v>19</v>
       </c>
       <c r="E155" t="n">
-        <v>90.164533820841</v>
+        <v>100</v>
       </c>
       <c r="F155" t="n">
         <v>0</v>
@@ -25666,7 +25666,7 @@
         <v>19</v>
       </c>
       <c r="E157" t="n">
-        <v>15.6706507304117</v>
+        <v>20.5699020480855</v>
       </c>
       <c r="F157" t="n">
         <v>0</v>
@@ -25698,7 +25698,7 @@
         <v>19</v>
       </c>
       <c r="E158" t="n">
-        <v>72.9083665338645</v>
+        <v>77.1148708815672</v>
       </c>
       <c r="F158" t="n">
         <v>0</v>
@@ -25730,7 +25730,7 @@
         <v>19</v>
       </c>
       <c r="E159" t="n">
-        <v>75.1660026560425</v>
+        <v>86.9991095280499</v>
       </c>
       <c r="F159" t="n">
         <v>0</v>
@@ -25762,7 +25762,7 @@
         <v>19</v>
       </c>
       <c r="E160" t="n">
-        <v>88.1806108897742</v>
+        <v>92.6090828138914</v>
       </c>
       <c r="F160" t="n">
         <v>0</v>
@@ -25794,7 +25794,7 @@
         <v>19</v>
       </c>
       <c r="E161" t="n">
-        <v>95.7503320053121</v>
+        <v>93.9447907390917</v>
       </c>
       <c r="F161" t="n">
         <v>0</v>
@@ -25826,7 +25826,7 @@
         <v>19</v>
       </c>
       <c r="E162" t="n">
-        <v>100</v>
+        <v>96.9723953695459</v>
       </c>
       <c r="F162" t="n">
         <v>0</v>
@@ -25890,7 +25890,7 @@
         <v>19</v>
       </c>
       <c r="E164" t="n">
-        <v>30.9668212629326</v>
+        <v>26.7206477732794</v>
       </c>
       <c r="F164" t="n">
         <v>0</v>
@@ -25922,7 +25922,7 @@
         <v>19</v>
       </c>
       <c r="E165" t="n">
-        <v>80.3781662504459</v>
+        <v>61.4372469635627</v>
       </c>
       <c r="F165" t="n">
         <v>0</v>
@@ -25954,7 +25954,7 @@
         <v>19</v>
       </c>
       <c r="E166" t="n">
-        <v>88.3696039957189</v>
+        <v>76.9230769230769</v>
       </c>
       <c r="F166" t="n">
         <v>0</v>
@@ -25986,7 +25986,7 @@
         <v>19</v>
       </c>
       <c r="E167" t="n">
-        <v>91.6874777024616</v>
+        <v>87.5506072874494</v>
       </c>
       <c r="F167" t="n">
         <v>0</v>
@@ -26018,7 +26018,7 @@
         <v>19</v>
       </c>
       <c r="E168" t="n">
-        <v>91.9728861933643</v>
+        <v>88.9676113360324</v>
       </c>
       <c r="F168" t="n">
         <v>0</v>
@@ -26050,7 +26050,7 @@
         <v>19</v>
       </c>
       <c r="E169" t="n">
-        <v>96.0756332500892</v>
+        <v>95.3441295546559</v>
       </c>
       <c r="F169" t="n">
         <v>0</v>
@@ -26114,7 +26114,7 @@
         <v>19</v>
       </c>
       <c r="E171" t="n">
-        <v>18.2905225863596</v>
+        <v>13.1161007667032</v>
       </c>
       <c r="F171" t="n">
         <v>0</v>
@@ -26146,7 +26146,7 @@
         <v>19</v>
       </c>
       <c r="E172" t="n">
-        <v>72.7635075287865</v>
+        <v>27.1084337349398</v>
       </c>
       <c r="F172" t="n">
         <v>0</v>
@@ -26178,7 +26178,7 @@
         <v>19</v>
       </c>
       <c r="E173" t="n">
-        <v>79.362267493357</v>
+        <v>60.2135815991238</v>
       </c>
       <c r="F173" t="n">
         <v>0</v>
@@ -26210,7 +26210,7 @@
         <v>19</v>
       </c>
       <c r="E174" t="n">
-        <v>90.4340124003543</v>
+        <v>76.7798466593647</v>
       </c>
       <c r="F174" t="n">
         <v>0</v>
@@ -26242,7 +26242,7 @@
         <v>19</v>
       </c>
       <c r="E175" t="n">
-        <v>100</v>
+        <v>82.9956188389923</v>
       </c>
       <c r="F175" t="n">
         <v>0</v>
@@ -26274,7 +26274,7 @@
         <v>19</v>
       </c>
       <c r="E176" t="n">
-        <v>100</v>
+        <v>92.579408543264</v>
       </c>
       <c r="F176" t="n">
         <v>0</v>
@@ -26338,7 +26338,7 @@
         <v>19</v>
       </c>
       <c r="E178" t="n">
-        <v>14.6772228989038</v>
+        <v>15.2752009894867</v>
       </c>
       <c r="F178" t="n">
         <v>0</v>
@@ -26370,7 +26370,7 @@
         <v>19</v>
       </c>
       <c r="E179" t="n">
-        <v>22.5943970767357</v>
+        <v>35.9925788497217</v>
       </c>
       <c r="F179" t="n">
         <v>0</v>
@@ -26402,7 +26402,7 @@
         <v>19</v>
       </c>
       <c r="E180" t="n">
-        <v>59.3788063337393</v>
+        <v>78.9734075448361</v>
       </c>
       <c r="F180" t="n">
         <v>0</v>
@@ -26434,7 +26434,7 @@
         <v>19</v>
       </c>
       <c r="E181" t="n">
-        <v>83.373934226553</v>
+        <v>82.9931972789116</v>
       </c>
       <c r="F181" t="n">
         <v>0</v>
@@ -26466,7 +26466,7 @@
         <v>19</v>
       </c>
       <c r="E182" t="n">
-        <v>88.5809987819732</v>
+        <v>86.2708719851577</v>
       </c>
       <c r="F182" t="n">
         <v>0</v>
@@ -26498,7 +26498,7 @@
         <v>19</v>
       </c>
       <c r="E183" t="n">
-        <v>91.5956151035323</v>
+        <v>88.9919604205318</v>
       </c>
       <c r="F183" t="n">
         <v>0</v>
@@ -26562,7 +26562,7 @@
         <v>19</v>
       </c>
       <c r="E185" t="n">
-        <v>19.5777351247601</v>
+        <v>4.88155061019383</v>
       </c>
       <c r="F185" t="n">
         <v>0</v>
@@ -26594,7 +26594,7 @@
         <v>19</v>
       </c>
       <c r="E186" t="n">
-        <v>51.1996161228407</v>
+        <v>12.275664034458</v>
       </c>
       <c r="F186" t="n">
         <v>0</v>
@@ -26626,7 +26626,7 @@
         <v>19</v>
       </c>
       <c r="E187" t="n">
-        <v>69.4817658349328</v>
+        <v>40.9906676238335</v>
       </c>
       <c r="F187" t="n">
         <v>0</v>
@@ -26658,7 +26658,7 @@
         <v>19</v>
       </c>
       <c r="E188" t="n">
-        <v>78.5988483685221</v>
+        <v>61.4860014357502</v>
       </c>
       <c r="F188" t="n">
         <v>0</v>
@@ -26690,7 +26690,7 @@
         <v>19</v>
       </c>
       <c r="E189" t="n">
-        <v>85.1727447216891</v>
+        <v>74.5872218234027</v>
       </c>
       <c r="F189" t="n">
         <v>0</v>
@@ -26722,7 +26722,7 @@
         <v>19</v>
       </c>
       <c r="E190" t="n">
-        <v>91.2667946257198</v>
+        <v>87.8679109834889</v>
       </c>
       <c r="F190" t="n">
         <v>0</v>
@@ -26786,7 +26786,7 @@
         <v>19</v>
       </c>
       <c r="E192" t="n">
-        <v>26.7925561029009</v>
+        <v>38.6872455902307</v>
       </c>
       <c r="F192" t="n">
         <v>0</v>
@@ -26818,7 +26818,7 @@
         <v>19</v>
       </c>
       <c r="E193" t="n">
-        <v>89.983579638752</v>
+        <v>87.1947082767978</v>
       </c>
       <c r="F193" t="n">
         <v>0</v>
@@ -26850,7 +26850,7 @@
         <v>19</v>
       </c>
       <c r="E194" t="n">
-        <v>94.1981390257252</v>
+        <v>92.9952510176391</v>
       </c>
       <c r="F194" t="n">
         <v>0</v>
@@ -26882,7 +26882,7 @@
         <v>19</v>
       </c>
       <c r="E195" t="n">
-        <v>95.1833607006021</v>
+        <v>93.9959294436906</v>
       </c>
       <c r="F195" t="n">
         <v>0</v>
@@ -26914,7 +26914,7 @@
         <v>19</v>
       </c>
       <c r="E196" t="n">
-        <v>96.9896004378763</v>
+        <v>96.9810040705563</v>
       </c>
       <c r="F196" t="n">
         <v>0</v>
@@ -26946,7 +26946,7 @@
         <v>19</v>
       </c>
       <c r="E197" t="n">
-        <v>97.4822112753147</v>
+        <v>100</v>
       </c>
       <c r="F197" t="n">
         <v>0</v>
@@ -27010,7 +27010,7 @@
         <v>19</v>
       </c>
       <c r="E199" t="n">
-        <v>30.0678221552374</v>
+        <v>29.0849673202614</v>
       </c>
       <c r="F199" t="n">
         <v>0</v>
@@ -27042,7 +27042,7 @@
         <v>19</v>
       </c>
       <c r="E200" t="n">
-        <v>66.46571213263</v>
+        <v>76.1801016702977</v>
       </c>
       <c r="F200" t="n">
         <v>0</v>
@@ -27074,7 +27074,7 @@
         <v>19</v>
       </c>
       <c r="E201" t="n">
-        <v>87.3398643556895</v>
+        <v>90.7770515613653</v>
       </c>
       <c r="F201" t="n">
         <v>0</v>
@@ -27106,7 +27106,7 @@
         <v>19</v>
       </c>
       <c r="E202" t="n">
-        <v>88.2441597588546</v>
+        <v>91.3943355119826</v>
       </c>
       <c r="F202" t="n">
         <v>0</v>
@@ -27138,7 +27138,7 @@
         <v>19</v>
       </c>
       <c r="E203" t="n">
-        <v>88.5455915599096</v>
+        <v>97.9665940450254</v>
       </c>
       <c r="F203" t="n">
         <v>0</v>
@@ -27170,7 +27170,7 @@
         <v>19</v>
       </c>
       <c r="E204" t="n">
-        <v>94.9510173323286</v>
+        <v>100</v>
       </c>
       <c r="F204" t="n">
         <v>0</v>
@@ -27234,7 +27234,7 @@
         <v>19</v>
       </c>
       <c r="E206" t="n">
-        <v>27.7358490566038</v>
+        <v>19.9664429530201</v>
       </c>
       <c r="F206" t="n">
         <v>0</v>
@@ -27266,7 +27266,7 @@
         <v>19</v>
       </c>
       <c r="E207" t="n">
-        <v>70.9905660377358</v>
+        <v>80.8724832214765</v>
       </c>
       <c r="F207" t="n">
         <v>0</v>
@@ -27298,7 +27298,7 @@
         <v>19</v>
       </c>
       <c r="E208" t="n">
-        <v>82.5943396226415</v>
+        <v>91.5268456375839</v>
       </c>
       <c r="F208" t="n">
         <v>0</v>
@@ -27330,7 +27330,7 @@
         <v>19</v>
       </c>
       <c r="E209" t="n">
-        <v>85.377358490566</v>
+        <v>91.988255033557</v>
       </c>
       <c r="F209" t="n">
         <v>0</v>
@@ -27362,7 +27362,7 @@
         <v>19</v>
       </c>
       <c r="E210" t="n">
-        <v>97.3584905660377</v>
+        <v>96.9798657718121</v>
       </c>
       <c r="F210" t="n">
         <v>0</v>
@@ -27394,7 +27394,7 @@
         <v>19</v>
       </c>
       <c r="E211" t="n">
-        <v>98.8679245283019</v>
+        <v>100</v>
       </c>
       <c r="F211" t="n">
         <v>0</v>
@@ -27458,7 +27458,7 @@
         <v>20</v>
       </c>
       <c r="E213" t="n">
-        <v>10.1608806096528</v>
+        <v>18.4673366834171</v>
       </c>
       <c r="F213" t="n">
         <v>1</v>
@@ -27490,7 +27490,7 @@
         <v>20</v>
       </c>
       <c r="E214" t="n">
-        <v>15.8340389500423</v>
+        <v>95.3517587939699</v>
       </c>
       <c r="F214" t="n">
         <v>1</v>
@@ -27522,7 +27522,7 @@
         <v>20</v>
       </c>
       <c r="E215" t="n">
-        <v>96.8670618120237</v>
+        <v>97.2361809045226</v>
       </c>
       <c r="F215" t="n">
         <v>1</v>
@@ -27554,7 +27554,7 @@
         <v>20</v>
       </c>
       <c r="E216" t="n">
-        <v>97.6291278577477</v>
+        <v>98.2412060301507</v>
       </c>
       <c r="F216" t="n">
         <v>1</v>
@@ -27586,7 +27586,7 @@
         <v>20</v>
       </c>
       <c r="E217" t="n">
-        <v>98.1371718882303</v>
+        <v>100</v>
       </c>
       <c r="F217" t="n">
         <v>1</v>
@@ -27682,7 +27682,7 @@
         <v>20</v>
       </c>
       <c r="E220" t="n">
-        <v>21.280276816609</v>
+        <v>18.3948863636364</v>
       </c>
       <c r="F220" t="n">
         <v>1</v>
@@ -27714,7 +27714,7 @@
         <v>20</v>
       </c>
       <c r="E221" t="n">
-        <v>65.3979238754325</v>
+        <v>50.7102272727273</v>
       </c>
       <c r="F221" t="n">
         <v>1</v>
@@ -27746,7 +27746,7 @@
         <v>20</v>
       </c>
       <c r="E222" t="n">
-        <v>84.6020761245675</v>
+        <v>66.9744318181818</v>
       </c>
       <c r="F222" t="n">
         <v>1</v>
@@ -27778,7 +27778,7 @@
         <v>20</v>
       </c>
       <c r="E223" t="n">
-        <v>90.8304498269896</v>
+        <v>84.4460227272727</v>
       </c>
       <c r="F223" t="n">
         <v>1</v>
@@ -27810,7 +27810,7 @@
         <v>20</v>
       </c>
       <c r="E224" t="n">
-        <v>99.1349480968858</v>
+        <v>92.8267045454545</v>
       </c>
       <c r="F224" t="n">
         <v>1</v>
@@ -27842,7 +27842,7 @@
         <v>20</v>
       </c>
       <c r="E225" t="n">
-        <v>100</v>
+        <v>97.0880681818182</v>
       </c>
       <c r="F225" t="n">
         <v>1</v>
@@ -27906,7 +27906,7 @@
         <v>20</v>
       </c>
       <c r="E227" t="n">
-        <v>1.88679245283019</v>
+        <v>17.9271708683473</v>
       </c>
       <c r="F227" t="n">
         <v>1</v>
@@ -27938,7 +27938,7 @@
         <v>20</v>
       </c>
       <c r="E228" t="n">
-        <v>2.35849056603774</v>
+        <v>22.4789915966387</v>
       </c>
       <c r="F228" t="n">
         <v>1</v>
@@ -27970,7 +27970,7 @@
         <v>20</v>
       </c>
       <c r="E229" t="n">
-        <v>6.44654088050314</v>
+        <v>56.3725490196078</v>
       </c>
       <c r="F229" t="n">
         <v>1</v>
@@ -28002,7 +28002,7 @@
         <v>20</v>
       </c>
       <c r="E230" t="n">
-        <v>47.6415094339623</v>
+        <v>87.4649859943978</v>
       </c>
       <c r="F230" t="n">
         <v>1</v>
@@ -28034,7 +28034,7 @@
         <v>20</v>
       </c>
       <c r="E231" t="n">
-        <v>74.3710691823899</v>
+        <v>92.5070028011204</v>
       </c>
       <c r="F231" t="n">
         <v>1</v>
@@ -28066,7 +28066,7 @@
         <v>20</v>
       </c>
       <c r="E232" t="n">
-        <v>86.7924528301887</v>
+        <v>94.2577030812325</v>
       </c>
       <c r="F232" t="n">
         <v>1</v>
@@ -28130,7 +28130,7 @@
         <v>20</v>
       </c>
       <c r="E234" t="n">
-        <v>2.02966432474629</v>
+        <v>13.9621240252506</v>
       </c>
       <c r="F234" t="n">
         <v>0</v>
@@ -28162,7 +28162,7 @@
         <v>20</v>
       </c>
       <c r="E235" t="n">
-        <v>3.94223263075722</v>
+        <v>17.5269216487189</v>
       </c>
       <c r="F235" t="n">
         <v>0</v>
@@ -28194,7 +28194,7 @@
         <v>20</v>
       </c>
       <c r="E236" t="n">
-        <v>9.21155347384856</v>
+        <v>50.2413665057557</v>
       </c>
       <c r="F236" t="n">
         <v>0</v>
@@ -28226,7 +28226,7 @@
         <v>20</v>
       </c>
       <c r="E237" t="n">
-        <v>12.8805620608899</v>
+        <v>80.9877460081693</v>
       </c>
       <c r="F237" t="n">
         <v>0</v>
@@ -28258,7 +28258,7 @@
         <v>20</v>
       </c>
       <c r="E238" t="n">
-        <v>30.9914129586261</v>
+        <v>94.0215373189751</v>
       </c>
       <c r="F238" t="n">
         <v>0</v>
@@ -28290,7 +28290,7 @@
         <v>20</v>
       </c>
       <c r="E239" t="n">
-        <v>43.6377829820453</v>
+        <v>99.814333457111</v>
       </c>
       <c r="F239" t="n">
         <v>0</v>
@@ -28354,7 +28354,7 @@
         <v>20</v>
       </c>
       <c r="E241" t="n">
-        <v>13.9733840304183</v>
+        <v>21.1764705882353</v>
       </c>
       <c r="F241" t="n">
         <v>0</v>
@@ -28386,7 +28386,7 @@
         <v>20</v>
       </c>
       <c r="E242" t="n">
-        <v>24.287072243346</v>
+        <v>39.9396681749623</v>
       </c>
       <c r="F242" t="n">
         <v>0</v>
@@ -28418,7 +28418,7 @@
         <v>20</v>
       </c>
       <c r="E243" t="n">
-        <v>51.3783269961977</v>
+        <v>48.6877828054299</v>
       </c>
       <c r="F243" t="n">
         <v>0</v>
@@ -28450,7 +28450,7 @@
         <v>20</v>
       </c>
       <c r="E244" t="n">
-        <v>78.754752851711</v>
+        <v>61.6892911010558</v>
       </c>
       <c r="F244" t="n">
         <v>0</v>
@@ -28482,7 +28482,7 @@
         <v>20</v>
       </c>
       <c r="E245" t="n">
-        <v>88.3555133079848</v>
+        <v>81.3876319758673</v>
       </c>
       <c r="F245" t="n">
         <v>0</v>
@@ -28514,7 +28514,7 @@
         <v>20</v>
       </c>
       <c r="E246" t="n">
-        <v>94.9619771863118</v>
+        <v>91.1010558069382</v>
       </c>
       <c r="F246" t="n">
         <v>0</v>
@@ -28578,7 +28578,7 @@
         <v>20</v>
       </c>
       <c r="E248" t="n">
-        <v>7.54300838112042</v>
+        <v>23.8774055595153</v>
       </c>
       <c r="F248" t="n">
         <v>0</v>
@@ -28610,7 +28610,7 @@
         <v>20</v>
       </c>
       <c r="E249" t="n">
-        <v>24.0405822673136</v>
+        <v>70.6343549536707</v>
       </c>
       <c r="F249" t="n">
         <v>0</v>
@@ -28642,7 +28642,7 @@
         <v>20</v>
       </c>
       <c r="E250" t="n">
-        <v>39.5677106307896</v>
+        <v>93.5495367070563</v>
       </c>
       <c r="F250" t="n">
         <v>0</v>
@@ -28674,7 +28674,7 @@
         <v>20</v>
       </c>
       <c r="E251" t="n">
-        <v>66.2990736656374</v>
+        <v>99.1446899501069</v>
       </c>
       <c r="F251" t="n">
         <v>0</v>
@@ -28706,7 +28706,7 @@
         <v>20</v>
       </c>
       <c r="E252" t="n">
-        <v>83.5465372739303</v>
+        <v>99.1446899501069</v>
       </c>
       <c r="F252" t="n">
         <v>0</v>
@@ -28738,7 +28738,7 @@
         <v>20</v>
       </c>
       <c r="E253" t="n">
-        <v>87.5606528451698</v>
+        <v>100</v>
       </c>
       <c r="F253" t="n">
         <v>0</v>
@@ -28802,7 +28802,7 @@
         <v>20</v>
       </c>
       <c r="E255" t="n">
-        <v>23.4901568234902</v>
+        <v>18.5126582278481</v>
       </c>
       <c r="F255" t="n">
         <v>0</v>
@@ -28834,7 +28834,7 @@
         <v>20</v>
       </c>
       <c r="E256" t="n">
-        <v>76.4097430764097</v>
+        <v>65.0316455696203</v>
       </c>
       <c r="F256" t="n">
         <v>0</v>
@@ -28866,7 +28866,7 @@
         <v>20</v>
       </c>
       <c r="E257" t="n">
-        <v>76.4097430764097</v>
+        <v>80.2215189873418</v>
       </c>
       <c r="F257" t="n">
         <v>0</v>
@@ -28898,7 +28898,7 @@
         <v>20</v>
       </c>
       <c r="E258" t="n">
-        <v>78.2782782782783</v>
+        <v>84.1772151898734</v>
       </c>
       <c r="F258" t="n">
         <v>0</v>
@@ -28930,7 +28930,7 @@
         <v>20</v>
       </c>
       <c r="E259" t="n">
-        <v>82.6493159826493</v>
+        <v>97.1518987341772</v>
       </c>
       <c r="F259" t="n">
         <v>0</v>
@@ -28962,7 +28962,7 @@
         <v>20</v>
       </c>
       <c r="E260" t="n">
-        <v>91.5248581915249</v>
+        <v>100</v>
       </c>
       <c r="F260" t="n">
         <v>0</v>
@@ -29026,7 +29026,7 @@
         <v>20</v>
       </c>
       <c r="E262" t="n">
-        <v>15.8113730929265</v>
+        <v>21.9638242894057</v>
       </c>
       <c r="F262" t="n">
         <v>0</v>
@@ -29058,7 +29058,7 @@
         <v>20</v>
       </c>
       <c r="E263" t="n">
-        <v>75.1733703190014</v>
+        <v>80.275624461671</v>
       </c>
       <c r="F263" t="n">
         <v>0</v>
@@ -29090,7 +29090,7 @@
         <v>20</v>
       </c>
       <c r="E264" t="n">
-        <v>76.005547850208</v>
+        <v>88.8027562446167</v>
       </c>
       <c r="F264" t="n">
         <v>0</v>
@@ -29122,7 +29122,7 @@
         <v>20</v>
       </c>
       <c r="E265" t="n">
-        <v>87.6560332871013</v>
+        <v>92.2480620155039</v>
       </c>
       <c r="F265" t="n">
         <v>0</v>
@@ -29154,7 +29154,7 @@
         <v>20</v>
       </c>
       <c r="E266" t="n">
-        <v>96.25520110957</v>
+        <v>92.4203273040482</v>
       </c>
       <c r="F266" t="n">
         <v>0</v>
@@ -29186,7 +29186,7 @@
         <v>20</v>
       </c>
       <c r="E267" t="n">
-        <v>100</v>
+        <v>96.9853574504737</v>
       </c>
       <c r="F267" t="n">
         <v>0</v>
@@ -29250,7 +29250,7 @@
         <v>20</v>
       </c>
       <c r="E269" t="n">
-        <v>30.2517850432168</v>
+        <v>27.2641509433962</v>
       </c>
       <c r="F269" t="n">
         <v>0</v>
@@ -29282,7 +29282,7 @@
         <v>20</v>
       </c>
       <c r="E270" t="n">
-        <v>80.9470124013529</v>
+        <v>61.9811320754717</v>
       </c>
       <c r="F270" t="n">
         <v>0</v>
@@ -29314,7 +29314,7 @@
         <v>20</v>
       </c>
       <c r="E271" t="n">
-        <v>90.717775272454</v>
+        <v>75.8490566037736</v>
       </c>
       <c r="F271" t="n">
         <v>0</v>
@@ -29346,7 +29346,7 @@
         <v>20</v>
       </c>
       <c r="E272" t="n">
-        <v>93.2732055618189</v>
+        <v>87.8301886792453</v>
       </c>
       <c r="F272" t="n">
         <v>0</v>
@@ -29378,7 +29378,7 @@
         <v>20</v>
       </c>
       <c r="E273" t="n">
-        <v>93.3859451334085</v>
+        <v>89.2452830188679</v>
       </c>
       <c r="F273" t="n">
         <v>0</v>
@@ -29410,7 +29410,7 @@
         <v>20</v>
       </c>
       <c r="E274" t="n">
-        <v>94.7763998496806</v>
+        <v>95</v>
       </c>
       <c r="F274" t="n">
         <v>0</v>
@@ -29474,7 +29474,7 @@
         <v>20</v>
       </c>
       <c r="E276" t="n">
-        <v>18.3967112024666</v>
+        <v>14.7960415158098</v>
       </c>
       <c r="F276" t="n">
         <v>0</v>
@@ -29506,7 +29506,7 @@
         <v>20</v>
       </c>
       <c r="E277" t="n">
-        <v>71.4285714285714</v>
+        <v>34.2988172821627</v>
       </c>
       <c r="F277" t="n">
         <v>0</v>
@@ -29538,7 +29538,7 @@
         <v>20</v>
       </c>
       <c r="E278" t="n">
-        <v>81.7574511819116</v>
+        <v>61.0909968621772</v>
       </c>
       <c r="F278" t="n">
         <v>0</v>
@@ -29570,7 +29570,7 @@
         <v>20</v>
       </c>
       <c r="E279" t="n">
-        <v>91.2127440904419</v>
+        <v>75.8387641805455</v>
       </c>
       <c r="F279" t="n">
         <v>0</v>
@@ -29602,7 +29602,7 @@
         <v>20</v>
       </c>
       <c r="E280" t="n">
-        <v>100</v>
+        <v>83.2971276852522</v>
       </c>
       <c r="F280" t="n">
         <v>0</v>
@@ -29634,7 +29634,7 @@
         <v>20</v>
       </c>
       <c r="E281" t="n">
-        <v>100</v>
+        <v>92.3244026068067</v>
       </c>
       <c r="F281" t="n">
         <v>0</v>
@@ -29698,7 +29698,7 @@
         <v>20</v>
       </c>
       <c r="E283" t="n">
-        <v>12.8468033775633</v>
+        <v>15.0060753341434</v>
       </c>
       <c r="F283" t="n">
         <v>0</v>
@@ -29730,7 +29730,7 @@
         <v>20</v>
       </c>
       <c r="E284" t="n">
-        <v>21.2002412545235</v>
+        <v>40.1883353584447</v>
       </c>
       <c r="F284" t="n">
         <v>0</v>
@@ -29762,7 +29762,7 @@
         <v>20</v>
       </c>
       <c r="E285" t="n">
-        <v>61.7913148371532</v>
+        <v>79.9817739975699</v>
       </c>
       <c r="F285" t="n">
         <v>0</v>
@@ -29794,7 +29794,7 @@
         <v>20</v>
       </c>
       <c r="E286" t="n">
-        <v>82.4788902291918</v>
+        <v>82.0777642770352</v>
       </c>
       <c r="F286" t="n">
         <v>0</v>
@@ -29826,7 +29826,7 @@
         <v>20</v>
       </c>
       <c r="E287" t="n">
-        <v>88.8721351025332</v>
+        <v>84.6294046172539</v>
       </c>
       <c r="F287" t="n">
         <v>0</v>
@@ -29858,7 +29858,7 @@
         <v>20</v>
       </c>
       <c r="E288" t="n">
-        <v>91.8878166465621</v>
+        <v>91.9805589307412</v>
       </c>
       <c r="F288" t="n">
         <v>0</v>
@@ -29922,7 +29922,7 @@
         <v>20</v>
       </c>
       <c r="E290" t="n">
-        <v>19.3863939528679</v>
+        <v>4.09988818486769</v>
       </c>
       <c r="F290" t="n">
         <v>0</v>
@@ -29954,7 +29954,7 @@
         <v>20</v>
       </c>
       <c r="E291" t="n">
-        <v>52.9568697198755</v>
+        <v>13.2687290346627</v>
       </c>
       <c r="F291" t="n">
         <v>0</v>
@@ -29986,7 +29986,7 @@
         <v>20</v>
       </c>
       <c r="E292" t="n">
-        <v>67.718986216096</v>
+        <v>42.9370108087961</v>
       </c>
       <c r="F292" t="n">
         <v>0</v>
@@ -30018,7 +30018,7 @@
         <v>20</v>
       </c>
       <c r="E293" t="n">
-        <v>77.0120053357048</v>
+        <v>59.7838240775252</v>
       </c>
       <c r="F293" t="n">
         <v>0</v>
@@ -30050,7 +30050,7 @@
         <v>20</v>
       </c>
       <c r="E294" t="n">
-        <v>84.9710982658959</v>
+        <v>72.8289228475587</v>
       </c>
       <c r="F294" t="n">
         <v>0</v>
@@ -30082,7 +30082,7 @@
         <v>20</v>
       </c>
       <c r="E295" t="n">
-        <v>89.3730546909738</v>
+        <v>86.1349235929929</v>
       </c>
       <c r="F295" t="n">
         <v>0</v>
@@ -30146,7 +30146,7 @@
         <v>20</v>
       </c>
       <c r="E297" t="n">
-        <v>25.1535455053043</v>
+        <v>40.2679568291775</v>
       </c>
       <c r="F297" t="n">
         <v>0</v>
@@ -30178,7 +30178,7 @@
         <v>20</v>
       </c>
       <c r="E298" t="n">
-        <v>89.5030709101061</v>
+        <v>82.8433196873837</v>
       </c>
       <c r="F298" t="n">
         <v>0</v>
@@ -30210,7 +30210,7 @@
         <v>20</v>
       </c>
       <c r="E299" t="n">
-        <v>94.2769402568398</v>
+        <v>93.9337551172311</v>
       </c>
       <c r="F299" t="n">
         <v>0</v>
@@ -30242,7 +30242,7 @@
         <v>20</v>
       </c>
       <c r="E300" t="n">
-        <v>95.9240647682859</v>
+        <v>94.3431336062523</v>
       </c>
       <c r="F300" t="n">
         <v>0</v>
@@ -30274,7 +30274,7 @@
         <v>20</v>
       </c>
       <c r="E301" t="n">
-        <v>96.3149078726968</v>
+        <v>97.9903237811686</v>
       </c>
       <c r="F301" t="n">
         <v>0</v>
@@ -30306,7 +30306,7 @@
         <v>20</v>
       </c>
       <c r="E302" t="n">
-        <v>97.319932998325</v>
+        <v>100</v>
       </c>
       <c r="F302" t="n">
         <v>0</v>
@@ -30370,7 +30370,7 @@
         <v>20</v>
       </c>
       <c r="E304" t="n">
-        <v>30.2207130730051</v>
+        <v>29.3115942028986</v>
       </c>
       <c r="F304" t="n">
         <v>0</v>
@@ -30402,7 +30402,7 @@
         <v>20</v>
       </c>
       <c r="E305" t="n">
-        <v>65.365025466893</v>
+        <v>74.7826086956522</v>
       </c>
       <c r="F305" t="n">
         <v>0</v>
@@ -30434,7 +30434,7 @@
         <v>20</v>
       </c>
       <c r="E306" t="n">
-        <v>89.6434634974533</v>
+        <v>91.9565217391304</v>
       </c>
       <c r="F306" t="n">
         <v>0</v>
@@ -30466,7 +30466,7 @@
         <v>20</v>
       </c>
       <c r="E307" t="n">
-        <v>90.0679117147708</v>
+        <v>92.463768115942</v>
       </c>
       <c r="F307" t="n">
         <v>0</v>
@@ -30498,7 +30498,7 @@
         <v>20</v>
       </c>
       <c r="E308" t="n">
-        <v>91.0016977928693</v>
+        <v>96.268115942029</v>
       </c>
       <c r="F308" t="n">
         <v>0</v>
@@ -30530,7 +30530,7 @@
         <v>20</v>
       </c>
       <c r="E309" t="n">
-        <v>95.3310696095076</v>
+        <v>100</v>
       </c>
       <c r="F309" t="n">
         <v>0</v>
@@ -30594,7 +30594,7 @@
         <v>20</v>
       </c>
       <c r="E311" t="n">
-        <v>29.6761720637989</v>
+        <v>18.1034482758621</v>
       </c>
       <c r="F311" t="n">
         <v>0</v>
@@ -30626,7 +30626,7 @@
         <v>20</v>
       </c>
       <c r="E312" t="n">
-        <v>68.9705171580474</v>
+        <v>78.8362068965517</v>
       </c>
       <c r="F312" t="n">
         <v>0</v>
@@ -30658,7 +30658,7 @@
         <v>20</v>
       </c>
       <c r="E313" t="n">
-        <v>82.5036249395843</v>
+        <v>91.9827586206897</v>
       </c>
       <c r="F313" t="n">
         <v>0</v>
@@ -30690,7 +30690,7 @@
         <v>20</v>
       </c>
       <c r="E314" t="n">
-        <v>93.7167713871436</v>
+        <v>92.3706896551724</v>
       </c>
       <c r="F314" t="n">
         <v>0</v>
@@ -30722,7 +30722,7 @@
         <v>20</v>
       </c>
       <c r="E315" t="n">
-        <v>96.4233929434509</v>
+        <v>98.2758620689655</v>
       </c>
       <c r="F315" t="n">
         <v>0</v>
@@ -30754,7 +30754,7 @@
         <v>20</v>
       </c>
       <c r="E316" t="n">
-        <v>98.9850169163847</v>
+        <v>100</v>
       </c>
       <c r="F316" t="n">
         <v>0</v>

</xml_diff>